<commit_message>
Add Most popular StackOverflow tags in 3Q 2020
</commit_message>
<xml_diff>
--- a/results/rank-changes.xlsx
+++ b/results/rank-changes.xlsx
@@ -9,11 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="20201Q" sheetId="1" r:id="rId1"/>
     <sheet name="20202Q" sheetId="2" r:id="rId2"/>
+    <sheet name="20203Q" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="114">
   <si>
     <t>Tag</t>
   </si>
@@ -351,10 +352,22 @@
     <t>Rank 1Q</t>
   </si>
   <si>
-    <t>Rank Change</t>
-  </si>
-  <si>
     <t>Rank Changes</t>
+  </si>
+  <si>
+    <t>RANK</t>
+  </si>
+  <si>
+    <t>mongoose</t>
+  </si>
+  <si>
+    <t>datetime</t>
+  </si>
+  <si>
+    <t>discord</t>
+  </si>
+  <si>
+    <t>Rank 2Q</t>
   </si>
 </sst>
 </file>
@@ -676,10 +689,13 @@
   <dimension ref="A1:B101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -1498,13 +1514,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="4" max="5" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1521,7 +1538,7 @@
         <v>108</v>
       </c>
       <c r="E1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -3513,6 +3530,2042 @@
       </c>
       <c r="C101" t="e">
         <f>VLOOKUP(A101, '20201Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D101" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>VLOOKUP(A2, '20202Q'!A:B, 2, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(ISNA(D2), "new", IF(D2 = 0, "-", IF(D2 &gt; 0, CONCATENATE("u ", D2),   IF(D2 &lt; 0, CONCATENATE("d ", ABS(D2))))))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>VLOOKUP(A3, '20202Q'!A:B, 2, FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E66" si="1">IF(ISNA(D3), "new", IF(D3 = 0, "-", IF(D3 &gt; 0, CONCATENATE("u ", D3),   IF(D3 &lt; 0, CONCATENATE("d ", ABS(D3))))))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>VLOOKUP(A4, '20202Q'!A:B, 2, FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>VLOOKUP(A5, '20202Q'!A:B, 2, FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>VLOOKUP(A6, '20202Q'!A:B, 2, FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>VLOOKUP(A7, '20202Q'!A:B, 2, FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f>VLOOKUP(A8, '20202Q'!A:B, 2, FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f>VLOOKUP(A9, '20202Q'!A:B, 2, FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f>VLOOKUP(A10, '20202Q'!A:B, 2, FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f>VLOOKUP(A11, '20202Q'!A:B, 2, FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <f>VLOOKUP(A12, '20202Q'!A:B, 2, FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f>VLOOKUP(A13, '20202Q'!A:B, 2, FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f>VLOOKUP(A14, '20202Q'!A:B, 2, FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <f>VLOOKUP(A15, '20202Q'!A:B, 2, FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <f>VLOOKUP(A16, '20202Q'!A:B, 2, FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <f>VLOOKUP(A17, '20202Q'!A:B, 2, FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f>VLOOKUP(A18, '20202Q'!A:B, 2, FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <f>VLOOKUP(A19, '20202Q'!A:B, 2, FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f>VLOOKUP(A20, '20202Q'!A:B, 2, FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f>VLOOKUP(A21, '20202Q'!A:B, 2, FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <f>VLOOKUP(A22, '20202Q'!A:B, 2, FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f>VLOOKUP(A23, '20202Q'!A:B, 2, FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <f>VLOOKUP(A24, '20202Q'!A:B, 2, FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <f>VLOOKUP(A25, '20202Q'!A:B, 2, FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f>VLOOKUP(A26, '20202Q'!A:B, 2, FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <f>VLOOKUP(A27, '20202Q'!A:B, 2, FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <f>VLOOKUP(A28, '20202Q'!A:B, 2, FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <f>VLOOKUP(A29, '20202Q'!A:B, 2, FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>38</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <f>VLOOKUP(A30, '20202Q'!A:B, 2, FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <f>VLOOKUP(A31, '20202Q'!A:B, 2, FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <f>VLOOKUP(A32, '20202Q'!A:B, 2, FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <f>VLOOKUP(A33, '20202Q'!A:B, 2, FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <f>VLOOKUP(A34, '20202Q'!A:B, 2, FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>33</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <f>VLOOKUP(A35, '20202Q'!A:B, 2, FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>30</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <f>VLOOKUP(A36, '20202Q'!A:B, 2, FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <f>VLOOKUP(A37, '20202Q'!A:B, 2, FALSE)</f>
+        <v>36</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <f>VLOOKUP(A38, '20202Q'!A:B, 2, FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <f>VLOOKUP(A39, '20202Q'!A:B, 2, FALSE)</f>
+        <v>37</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <f>VLOOKUP(A40, '20202Q'!A:B, 2, FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <f>VLOOKUP(A41, '20202Q'!A:B, 2, FALSE)</f>
+        <v>42</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <f>VLOOKUP(A42, '20202Q'!A:B, 2, FALSE)</f>
+        <v>44</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <f>VLOOKUP(A43, '20202Q'!A:B, 2, FALSE)</f>
+        <v>38</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="1"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <f>VLOOKUP(A44, '20202Q'!A:B, 2, FALSE)</f>
+        <v>46</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>41</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <f>VLOOKUP(A45, '20202Q'!A:B, 2, FALSE)</f>
+        <v>41</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <f>VLOOKUP(A46, '20202Q'!A:B, 2, FALSE)</f>
+        <v>48</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>51</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <f>VLOOKUP(A47, '20202Q'!A:B, 2, FALSE)</f>
+        <v>47</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>52</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <f>VLOOKUP(A48, '20202Q'!A:B, 2, FALSE)</f>
+        <v>49</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <f>VLOOKUP(A49, '20202Q'!A:B, 2, FALSE)</f>
+        <v>45</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <f>VLOOKUP(A50, '20202Q'!A:B, 2, FALSE)</f>
+        <v>43</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="1"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>49</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <f>VLOOKUP(A51, '20202Q'!A:B, 2, FALSE)</f>
+        <v>52</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>63</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <f>VLOOKUP(A52, '20202Q'!A:B, 2, FALSE)</f>
+        <v>58</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="1"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>61</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <f>VLOOKUP(A53, '20202Q'!A:B, 2, FALSE)</f>
+        <v>59</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="1"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <f>VLOOKUP(A54, '20202Q'!A:B, 2, FALSE)</f>
+        <v>53</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <f>VLOOKUP(A55, '20202Q'!A:B, 2, FALSE)</f>
+        <v>54</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <f>VLOOKUP(A56, '20202Q'!A:B, 2, FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <f>VLOOKUP(A57, '20202Q'!A:B, 2, FALSE)</f>
+        <v>60</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="1"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>66</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <f>VLOOKUP(A58, '20202Q'!A:B, 2, FALSE)</f>
+        <v>57</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59">
+        <f>VLOOKUP(A59, '20202Q'!A:B, 2, FALSE)</f>
+        <v>61</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <f>VLOOKUP(A60, '20202Q'!A:B, 2, FALSE)</f>
+        <v>55</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="1"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>55</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61">
+        <f>VLOOKUP(A61, '20202Q'!A:B, 2, FALSE)</f>
+        <v>51</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>-9</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="1"/>
+        <v>d 9</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>65</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62">
+        <f>VLOOKUP(A62, '20202Q'!A:B, 2, FALSE)</f>
+        <v>68</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="1"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>54</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+      <c r="C63">
+        <f>VLOOKUP(A63, '20202Q'!A:B, 2, FALSE)</f>
+        <v>56</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="1"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>91</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+      <c r="C64">
+        <f>VLOOKUP(A64, '20202Q'!A:B, 2, FALSE)</f>
+        <v>66</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>86</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65">
+        <f>VLOOKUP(A65, '20202Q'!A:B, 2, FALSE)</f>
+        <v>63</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="C66">
+        <f>VLOOKUP(A66, '20202Q'!A:B, 2, FALSE)</f>
+        <v>81</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="1"/>
+        <v>u 16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+      <c r="C67">
+        <f>VLOOKUP(A67, '20202Q'!A:B, 2, FALSE)</f>
+        <v>65</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D101" si="2">C67-B67</f>
+        <v>-1</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" ref="E67:E101" si="3">IF(ISNA(D67), "new", IF(D67 = 0, "-", IF(D67 &gt; 0, CONCATENATE("u ", D67),   IF(D67 &lt; 0, CONCATENATE("d ", ABS(D67))))))</f>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>64</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68">
+        <f>VLOOKUP(A68, '20202Q'!A:B, 2, FALSE)</f>
+        <v>64</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="3"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>90</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69">
+        <f>VLOOKUP(A69, '20202Q'!A:B, 2, FALSE)</f>
+        <v>77</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="3"/>
+        <v>u 9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>62</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70">
+        <f>VLOOKUP(A70, '20202Q'!A:B, 2, FALSE)</f>
+        <v>72</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="3"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>77</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71">
+        <f>VLOOKUP(A71, '20202Q'!A:B, 2, FALSE)</f>
+        <v>73</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="3"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72">
+        <f>VLOOKUP(A72, '20202Q'!A:B, 2, FALSE)</f>
+        <v>62</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="3"/>
+        <v>d 9</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+      <c r="C73">
+        <f>VLOOKUP(A73, '20202Q'!A:B, 2, FALSE)</f>
+        <v>67</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="3"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>67</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+      <c r="C74">
+        <f>VLOOKUP(A74, '20202Q'!A:B, 2, FALSE)</f>
+        <v>71</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>68</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+      <c r="C75">
+        <f>VLOOKUP(A75, '20202Q'!A:B, 2, FALSE)</f>
+        <v>78</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="3"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>74</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+      <c r="C76">
+        <f>VLOOKUP(A76, '20202Q'!A:B, 2, FALSE)</f>
+        <v>75</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+      <c r="C77">
+        <f>VLOOKUP(A77, '20202Q'!A:B, 2, FALSE)</f>
+        <v>70</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="2"/>
+        <v>-6</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="3"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>73</v>
+      </c>
+      <c r="B78">
+        <v>77</v>
+      </c>
+      <c r="C78">
+        <f>VLOOKUP(A78, '20202Q'!A:B, 2, FALSE)</f>
+        <v>69</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="3"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>103</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+      <c r="C79">
+        <f>VLOOKUP(A79, '20202Q'!A:B, 2, FALSE)</f>
+        <v>96</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="2"/>
+        <v>18</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="3"/>
+        <v>u 18</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>70</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+      <c r="C80">
+        <f>VLOOKUP(A80, '20202Q'!A:B, 2, FALSE)</f>
+        <v>74</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="3"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>84</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+      <c r="C81">
+        <f>VLOOKUP(A81, '20202Q'!A:B, 2, FALSE)</f>
+        <v>76</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="3"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>85</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+      <c r="C82">
+        <f>VLOOKUP(A82, '20202Q'!A:B, 2, FALSE)</f>
+        <v>88</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="3"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>100</v>
+      </c>
+      <c r="B83">
+        <v>82</v>
+      </c>
+      <c r="C83">
+        <f>VLOOKUP(A83, '20202Q'!A:B, 2, FALSE)</f>
+        <v>86</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="3"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>95</v>
+      </c>
+      <c r="B84">
+        <v>83</v>
+      </c>
+      <c r="C84">
+        <f>VLOOKUP(A84, '20202Q'!A:B, 2, FALSE)</f>
+        <v>80</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="3"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85">
+        <v>84</v>
+      </c>
+      <c r="C85">
+        <f>VLOOKUP(A85, '20202Q'!A:B, 2, FALSE)</f>
+        <v>91</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="3"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>83</v>
+      </c>
+      <c r="B86">
+        <v>85</v>
+      </c>
+      <c r="C86">
+        <f>VLOOKUP(A86, '20202Q'!A:B, 2, FALSE)</f>
+        <v>79</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="2"/>
+        <v>-6</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="3"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>82</v>
+      </c>
+      <c r="B87">
+        <v>86</v>
+      </c>
+      <c r="C87">
+        <f>VLOOKUP(A87, '20202Q'!A:B, 2, FALSE)</f>
+        <v>84</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>79</v>
+      </c>
+      <c r="B88">
+        <v>87</v>
+      </c>
+      <c r="C88">
+        <f>VLOOKUP(A88, '20202Q'!A:B, 2, FALSE)</f>
+        <v>83</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="3"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>93</v>
+      </c>
+      <c r="B89">
+        <v>88</v>
+      </c>
+      <c r="C89">
+        <f>VLOOKUP(A89, '20202Q'!A:B, 2, FALSE)</f>
+        <v>87</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="3"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>92</v>
+      </c>
+      <c r="B90">
+        <v>89</v>
+      </c>
+      <c r="C90">
+        <f>VLOOKUP(A90, '20202Q'!A:B, 2, FALSE)</f>
+        <v>92</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="3"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>80</v>
+      </c>
+      <c r="B91">
+        <v>90</v>
+      </c>
+      <c r="C91">
+        <f>VLOOKUP(A91, '20202Q'!A:B, 2, FALSE)</f>
+        <v>90</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>76</v>
+      </c>
+      <c r="B92">
+        <v>91</v>
+      </c>
+      <c r="C92">
+        <f>VLOOKUP(A92, '20202Q'!A:B, 2, FALSE)</f>
+        <v>93</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="3"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93">
+        <v>92</v>
+      </c>
+      <c r="C93">
+        <f>VLOOKUP(A93, '20202Q'!A:B, 2, FALSE)</f>
+        <v>94</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="3"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>81</v>
+      </c>
+      <c r="B94">
+        <v>93</v>
+      </c>
+      <c r="C94">
+        <f>VLOOKUP(A94, '20202Q'!A:B, 2, FALSE)</f>
+        <v>82</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="2"/>
+        <v>-11</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="3"/>
+        <v>d 11</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>110</v>
+      </c>
+      <c r="B95">
+        <v>94</v>
+      </c>
+      <c r="C95" t="e">
+        <f>VLOOKUP(A95, '20202Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D95" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E95" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>106</v>
+      </c>
+      <c r="B96">
+        <v>95</v>
+      </c>
+      <c r="C96">
+        <f>VLOOKUP(A96, '20202Q'!A:B, 2, FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>88</v>
+      </c>
+      <c r="B97">
+        <v>96</v>
+      </c>
+      <c r="C97">
+        <f>VLOOKUP(A97, '20202Q'!A:B, 2, FALSE)</f>
+        <v>95</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="3"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>111</v>
+      </c>
+      <c r="B98">
+        <v>97</v>
+      </c>
+      <c r="C98" t="e">
+        <f>VLOOKUP(A98, '20202Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D98" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>98</v>
+      </c>
+      <c r="B99">
+        <v>98</v>
+      </c>
+      <c r="C99" t="e">
+        <f>VLOOKUP(A99, '20202Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D99" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>78</v>
+      </c>
+      <c r="B100">
+        <v>99</v>
+      </c>
+      <c r="C100">
+        <f>VLOOKUP(A100, '20202Q'!A:B, 2, FALSE)</f>
+        <v>99</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>112</v>
+      </c>
+      <c r="B101">
+        <v>100</v>
+      </c>
+      <c r="C101" t="e">
+        <f>VLOOKUP(A101, '20202Q'!A:B, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D101" t="e">

</xml_diff>

<commit_message>
Add Most popular StackOverflow tags in 4Q 2020
</commit_message>
<xml_diff>
--- a/results/rank-changes.xlsx
+++ b/results/rank-changes.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="20201Q" sheetId="1" r:id="rId1"/>
     <sheet name="20202Q" sheetId="2" r:id="rId2"/>
     <sheet name="20203Q" sheetId="3" r:id="rId3"/>
+    <sheet name="20204Q" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="118">
   <si>
     <t>Tag</t>
   </si>
@@ -368,6 +369,18 @@
   </si>
   <si>
     <t>Rank 2Q</t>
+  </si>
+  <si>
+    <t>image</t>
+  </si>
+  <si>
+    <t>nginx</t>
+  </si>
+  <si>
+    <t>elasticsearch</t>
+  </si>
+  <si>
+    <t>Rank 3Q</t>
   </si>
 </sst>
 </file>
@@ -1515,7 +1528,7 @@
   <dimension ref="A1:E101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3550,8 +3563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView topLeftCell="A61" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5580,4 +5593,2042 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>VLOOKUP(A2, '20203Q'!A:B, 2, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(ISNA(D2), "new", IF(D2 = 0, "-", IF(D2 &gt; 0, CONCATENATE("u ", D2),   IF(D2 &lt; 0, CONCATENATE("d ", ABS(D2))))))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>VLOOKUP(A3, '20203Q'!A:B, 2, FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E66" si="1">IF(ISNA(D3), "new", IF(D3 = 0, "-", IF(D3 &gt; 0, CONCATENATE("u ", D3),   IF(D3 &lt; 0, CONCATENATE("d ", ABS(D3))))))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>VLOOKUP(A4, '20203Q'!A:B, 2, FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>VLOOKUP(A5, '20203Q'!A:B, 2, FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>VLOOKUP(A6, '20203Q'!A:B, 2, FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>VLOOKUP(A7, '20203Q'!A:B, 2, FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f>VLOOKUP(A8, '20203Q'!A:B, 2, FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f>VLOOKUP(A9, '20203Q'!A:B, 2, FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f>VLOOKUP(A10, '20203Q'!A:B, 2, FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f>VLOOKUP(A11, '20203Q'!A:B, 2, FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <f>VLOOKUP(A12, '20203Q'!A:B, 2, FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f>VLOOKUP(A13, '20203Q'!A:B, 2, FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f>VLOOKUP(A14, '20203Q'!A:B, 2, FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <f>VLOOKUP(A15, '20203Q'!A:B, 2, FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <f>VLOOKUP(A16, '20203Q'!A:B, 2, FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <f>VLOOKUP(A17, '20203Q'!A:B, 2, FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f>VLOOKUP(A18, '20203Q'!A:B, 2, FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <f>VLOOKUP(A19, '20203Q'!A:B, 2, FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>21</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f>VLOOKUP(A20, '20203Q'!A:B, 2, FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f>VLOOKUP(A21, '20203Q'!A:B, 2, FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <f>VLOOKUP(A22, '20203Q'!A:B, 2, FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>29</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f>VLOOKUP(A23, '20203Q'!A:B, 2, FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>u 8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <f>VLOOKUP(A24, '20203Q'!A:B, 2, FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <f>VLOOKUP(A25, '20203Q'!A:B, 2, FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f>VLOOKUP(A26, '20203Q'!A:B, 2, FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <f>VLOOKUP(A27, '20203Q'!A:B, 2, FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <f>VLOOKUP(A28, '20203Q'!A:B, 2, FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>34</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <f>VLOOKUP(A29, '20203Q'!A:B, 2, FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <f>VLOOKUP(A30, '20203Q'!A:B, 2, FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <f>VLOOKUP(A31, '20203Q'!A:B, 2, FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <f>VLOOKUP(A32, '20203Q'!A:B, 2, FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <f>VLOOKUP(A33, '20203Q'!A:B, 2, FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>28</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <f>VLOOKUP(A34, '20203Q'!A:B, 2, FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <f>VLOOKUP(A35, '20203Q'!A:B, 2, FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <f>VLOOKUP(A36, '20203Q'!A:B, 2, FALSE)</f>
+        <v>36</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <f>VLOOKUP(A37, '20203Q'!A:B, 2, FALSE)</f>
+        <v>37</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <f>VLOOKUP(A38, '20203Q'!A:B, 2, FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <f>VLOOKUP(A39, '20203Q'!A:B, 2, FALSE)</f>
+        <v>38</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>50</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <f>VLOOKUP(A40, '20203Q'!A:B, 2, FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <f>VLOOKUP(A41, '20203Q'!A:B, 2, FALSE)</f>
+        <v>43</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <f>VLOOKUP(A42, '20203Q'!A:B, 2, FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>49</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <f>VLOOKUP(A43, '20203Q'!A:B, 2, FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="1"/>
+        <v>u 8</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <f>VLOOKUP(A44, '20203Q'!A:B, 2, FALSE)</f>
+        <v>41</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <f>VLOOKUP(A45, '20203Q'!A:B, 2, FALSE)</f>
+        <v>47</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>51</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <f>VLOOKUP(A46, '20203Q'!A:B, 2, FALSE)</f>
+        <v>46</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <f>VLOOKUP(A47, '20203Q'!A:B, 2, FALSE)</f>
+        <v>49</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>46</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <f>VLOOKUP(A48, '20203Q'!A:B, 2, FALSE)</f>
+        <v>48</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>35</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <f>VLOOKUP(A49, '20203Q'!A:B, 2, FALSE)</f>
+        <v>42</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="1"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <f>VLOOKUP(A50, '20203Q'!A:B, 2, FALSE)</f>
+        <v>51</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <f>VLOOKUP(A51, '20203Q'!A:B, 2, FALSE)</f>
+        <v>45</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <f>VLOOKUP(A52, '20203Q'!A:B, 2, FALSE)</f>
+        <v>57</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="1"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <f>VLOOKUP(A53, '20203Q'!A:B, 2, FALSE)</f>
+        <v>55</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>60</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <f>VLOOKUP(A54, '20203Q'!A:B, 2, FALSE)</f>
+        <v>53</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>41</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <f>VLOOKUP(A55, '20203Q'!A:B, 2, FALSE)</f>
+        <v>44</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="1"/>
+        <v>d 10</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>61</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <f>VLOOKUP(A56, '20203Q'!A:B, 2, FALSE)</f>
+        <v>52</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>48</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <f>VLOOKUP(A57, '20203Q'!A:B, 2, FALSE)</f>
+        <v>54</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <f>VLOOKUP(A58, '20203Q'!A:B, 2, FALSE)</f>
+        <v>60</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59">
+        <f>VLOOKUP(A59, '20203Q'!A:B, 2, FALSE)</f>
+        <v>59</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>90</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <f>VLOOKUP(A60, '20203Q'!A:B, 2, FALSE)</f>
+        <v>68</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="1"/>
+        <v>u 9</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>71</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61">
+        <f>VLOOKUP(A61, '20203Q'!A:B, 2, FALSE)</f>
+        <v>71</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="1"/>
+        <v>u 11</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62">
+        <f>VLOOKUP(A62, '20203Q'!A:B, 2, FALSE)</f>
+        <v>58</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+      <c r="C63">
+        <f>VLOOKUP(A63, '20203Q'!A:B, 2, FALSE)</f>
+        <v>56</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="1"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>72</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+      <c r="C64">
+        <f>VLOOKUP(A64, '20203Q'!A:B, 2, FALSE)</f>
+        <v>66</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>54</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65">
+        <f>VLOOKUP(A65, '20203Q'!A:B, 2, FALSE)</f>
+        <v>62</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="C66">
+        <f>VLOOKUP(A66, '20203Q'!A:B, 2, FALSE)</f>
+        <v>61</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="1"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>89</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+      <c r="C67">
+        <f>VLOOKUP(A67, '20203Q'!A:B, 2, FALSE)</f>
+        <v>65</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D101" si="2">C67-B67</f>
+        <v>-1</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" ref="E67:E101" si="3">IF(ISNA(D67), "new", IF(D67 = 0, "-", IF(D67 &gt; 0, CONCATENATE("u ", D67),   IF(D67 &lt; 0, CONCATENATE("d ", ABS(D67))))))</f>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68">
+        <f>VLOOKUP(A68, '20203Q'!A:B, 2, FALSE)</f>
+        <v>73</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="3"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>73</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69">
+        <f>VLOOKUP(A69, '20203Q'!A:B, 2, FALSE)</f>
+        <v>77</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="3"/>
+        <v>u 9</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>64</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70">
+        <f>VLOOKUP(A70, '20203Q'!A:B, 2, FALSE)</f>
+        <v>67</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>74</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71">
+        <f>VLOOKUP(A71, '20203Q'!A:B, 2, FALSE)</f>
+        <v>75</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>62</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72">
+        <f>VLOOKUP(A72, '20203Q'!A:B, 2, FALSE)</f>
+        <v>69</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+      <c r="C73">
+        <f>VLOOKUP(A73, '20203Q'!A:B, 2, FALSE)</f>
+        <v>72</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>77</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+      <c r="C74">
+        <f>VLOOKUP(A74, '20203Q'!A:B, 2, FALSE)</f>
+        <v>70</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="3"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>69</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+      <c r="C75">
+        <f>VLOOKUP(A75, '20203Q'!A:B, 2, FALSE)</f>
+        <v>76</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="3"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>70</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+      <c r="C76">
+        <f>VLOOKUP(A76, '20203Q'!A:B, 2, FALSE)</f>
+        <v>79</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="3"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>68</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+      <c r="C77">
+        <f>VLOOKUP(A77, '20203Q'!A:B, 2, FALSE)</f>
+        <v>74</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>92</v>
+      </c>
+      <c r="B78">
+        <v>78</v>
+      </c>
+      <c r="C78">
+        <f>VLOOKUP(A78, '20203Q'!A:B, 2, FALSE)</f>
+        <v>89</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="2"/>
+        <v>11</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="3"/>
+        <v>u 11</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>86</v>
+      </c>
+      <c r="B79">
+        <v>77</v>
+      </c>
+      <c r="C79">
+        <f>VLOOKUP(A79, '20203Q'!A:B, 2, FALSE)</f>
+        <v>64</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="2"/>
+        <v>-13</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="3"/>
+        <v>d 13</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>84</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+      <c r="C80">
+        <f>VLOOKUP(A80, '20203Q'!A:B, 2, FALSE)</f>
+        <v>80</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="3"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>79</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+      <c r="C81">
+        <f>VLOOKUP(A81, '20203Q'!A:B, 2, FALSE)</f>
+        <v>87</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="3"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+      <c r="C82">
+        <f>VLOOKUP(A82, '20203Q'!A:B, 2, FALSE)</f>
+        <v>85</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="3"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>93</v>
+      </c>
+      <c r="B83">
+        <v>82</v>
+      </c>
+      <c r="C83">
+        <f>VLOOKUP(A83, '20203Q'!A:B, 2, FALSE)</f>
+        <v>88</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="3"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>82</v>
+      </c>
+      <c r="B84">
+        <v>83</v>
+      </c>
+      <c r="C84">
+        <f>VLOOKUP(A84, '20203Q'!A:B, 2, FALSE)</f>
+        <v>86</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="3"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>91</v>
+      </c>
+      <c r="B85">
+        <v>84</v>
+      </c>
+      <c r="C85">
+        <f>VLOOKUP(A85, '20203Q'!A:B, 2, FALSE)</f>
+        <v>63</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="2"/>
+        <v>-21</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="3"/>
+        <v>d 21</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>103</v>
+      </c>
+      <c r="B86">
+        <v>85</v>
+      </c>
+      <c r="C86">
+        <f>VLOOKUP(A86, '20203Q'!A:B, 2, FALSE)</f>
+        <v>78</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="2"/>
+        <v>-7</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="3"/>
+        <v>d 7</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>100</v>
+      </c>
+      <c r="B87">
+        <v>86</v>
+      </c>
+      <c r="C87">
+        <f>VLOOKUP(A87, '20203Q'!A:B, 2, FALSE)</f>
+        <v>82</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="3"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>75</v>
+      </c>
+      <c r="B88">
+        <v>87</v>
+      </c>
+      <c r="C88" t="e">
+        <f>VLOOKUP(A88, '20203Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D88" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>102</v>
+      </c>
+      <c r="B89">
+        <v>88</v>
+      </c>
+      <c r="C89" t="e">
+        <f>VLOOKUP(A89, '20203Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D89" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>80</v>
+      </c>
+      <c r="B90">
+        <v>89</v>
+      </c>
+      <c r="C90">
+        <f>VLOOKUP(A90, '20203Q'!A:B, 2, FALSE)</f>
+        <v>90</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="3"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>85</v>
+      </c>
+      <c r="B91">
+        <v>90</v>
+      </c>
+      <c r="C91">
+        <f>VLOOKUP(A91, '20203Q'!A:B, 2, FALSE)</f>
+        <v>81</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="3"/>
+        <v>d 9</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>96</v>
+      </c>
+      <c r="B92">
+        <v>91</v>
+      </c>
+      <c r="C92">
+        <f>VLOOKUP(A92, '20203Q'!A:B, 2, FALSE)</f>
+        <v>92</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="3"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>111</v>
+      </c>
+      <c r="B93">
+        <v>92</v>
+      </c>
+      <c r="C93">
+        <f>VLOOKUP(A93, '20203Q'!A:B, 2, FALSE)</f>
+        <v>97</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>110</v>
+      </c>
+      <c r="B94">
+        <v>93</v>
+      </c>
+      <c r="C94">
+        <f>VLOOKUP(A94, '20203Q'!A:B, 2, FALSE)</f>
+        <v>94</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="3"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>114</v>
+      </c>
+      <c r="B95">
+        <v>94</v>
+      </c>
+      <c r="C95" t="e">
+        <f>VLOOKUP(A95, '20203Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D95" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E95" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>112</v>
+      </c>
+      <c r="B96">
+        <v>95</v>
+      </c>
+      <c r="C96">
+        <f>VLOOKUP(A96, '20203Q'!A:B, 2, FALSE)</f>
+        <v>100</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>115</v>
+      </c>
+      <c r="B97">
+        <v>96</v>
+      </c>
+      <c r="C97" t="e">
+        <f>VLOOKUP(A97, '20203Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D97" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>99</v>
+      </c>
+      <c r="B98">
+        <v>97</v>
+      </c>
+      <c r="C98" t="e">
+        <f>VLOOKUP(A98, '20203Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D98" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>87</v>
+      </c>
+      <c r="B99">
+        <v>98</v>
+      </c>
+      <c r="C99">
+        <f>VLOOKUP(A99, '20203Q'!A:B, 2, FALSE)</f>
+        <v>84</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="2"/>
+        <v>-14</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="3"/>
+        <v>d 14</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>95</v>
+      </c>
+      <c r="B100">
+        <v>99</v>
+      </c>
+      <c r="C100">
+        <f>VLOOKUP(A100, '20203Q'!A:B, 2, FALSE)</f>
+        <v>83</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="2"/>
+        <v>-16</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="3"/>
+        <v>d 16</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>116</v>
+      </c>
+      <c r="B101">
+        <v>100</v>
+      </c>
+      <c r="C101" t="e">
+        <f>VLOOKUP(A101, '20203Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D101" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Most popular StackOverflow tags in 1Q 2021
</commit_message>
<xml_diff>
--- a/results/rank-changes.xlsx
+++ b/results/rank-changes.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="20201Q" sheetId="1" r:id="rId1"/>
     <sheet name="20202Q" sheetId="2" r:id="rId2"/>
     <sheet name="20203Q" sheetId="3" r:id="rId3"/>
     <sheet name="20204Q" sheetId="4" r:id="rId4"/>
+    <sheet name="20211Q" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="417" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="122">
   <si>
     <t>Tag</t>
   </si>
@@ -381,6 +382,18 @@
   </si>
   <si>
     <t>Rank 3Q</t>
+  </si>
+  <si>
+    <t>npm</t>
+  </si>
+  <si>
+    <t>discord.py</t>
+  </si>
+  <si>
+    <t>github</t>
+  </si>
+  <si>
+    <t>Rank 4Q</t>
   </si>
 </sst>
 </file>
@@ -5599,8 +5612,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -7631,4 +7644,2042 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>121</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>VLOOKUP(A2, '20204Q'!A:B, 2, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(ISNA(D2), "new", IF(D2 = 0, "-", IF(D2 &gt; 0, CONCATENATE("u ", D2),   IF(D2 &lt; 0, CONCATENATE("d ", ABS(D2))))))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>VLOOKUP(A3, '20204Q'!A:B, 2, FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E66" si="1">IF(ISNA(D3), "new", IF(D3 = 0, "-", IF(D3 &gt; 0, CONCATENATE("u ", D3),   IF(D3 &lt; 0, CONCATENATE("d ", ABS(D3))))))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>VLOOKUP(A4, '20204Q'!A:B, 2, FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>VLOOKUP(A5, '20204Q'!A:B, 2, FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>VLOOKUP(A6, '20204Q'!A:B, 2, FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>VLOOKUP(A7, '20204Q'!A:B, 2, FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f>VLOOKUP(A8, '20204Q'!A:B, 2, FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f>VLOOKUP(A9, '20204Q'!A:B, 2, FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f>VLOOKUP(A10, '20204Q'!A:B, 2, FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f>VLOOKUP(A11, '20204Q'!A:B, 2, FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <f>VLOOKUP(A12, '20204Q'!A:B, 2, FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f>VLOOKUP(A13, '20204Q'!A:B, 2, FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f>VLOOKUP(A14, '20204Q'!A:B, 2, FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <f>VLOOKUP(A15, '20204Q'!A:B, 2, FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <f>VLOOKUP(A16, '20204Q'!A:B, 2, FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <f>VLOOKUP(A17, '20204Q'!A:B, 2, FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f>VLOOKUP(A18, '20204Q'!A:B, 2, FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <f>VLOOKUP(A19, '20204Q'!A:B, 2, FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f>VLOOKUP(A20, '20204Q'!A:B, 2, FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f>VLOOKUP(A21, '20204Q'!A:B, 2, FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <f>VLOOKUP(A22, '20204Q'!A:B, 2, FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f>VLOOKUP(A23, '20204Q'!A:B, 2, FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <f>VLOOKUP(A24, '20204Q'!A:B, 2, FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>29</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <f>VLOOKUP(A25, '20204Q'!A:B, 2, FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f>VLOOKUP(A26, '20204Q'!A:B, 2, FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <f>VLOOKUP(A27, '20204Q'!A:B, 2, FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <f>VLOOKUP(A28, '20204Q'!A:B, 2, FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <f>VLOOKUP(A29, '20204Q'!A:B, 2, FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>34</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <f>VLOOKUP(A30, '20204Q'!A:B, 2, FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <f>VLOOKUP(A31, '20204Q'!A:B, 2, FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <f>VLOOKUP(A32, '20204Q'!A:B, 2, FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>31</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <f>VLOOKUP(A33, '20204Q'!A:B, 2, FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <f>VLOOKUP(A34, '20204Q'!A:B, 2, FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <f>VLOOKUP(A35, '20204Q'!A:B, 2, FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <f>VLOOKUP(A36, '20204Q'!A:B, 2, FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <f>VLOOKUP(A37, '20204Q'!A:B, 2, FALSE)</f>
+        <v>36</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>50</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <f>VLOOKUP(A38, '20204Q'!A:B, 2, FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <f>VLOOKUP(A39, '20204Q'!A:B, 2, FALSE)</f>
+        <v>38</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>30</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <f>VLOOKUP(A40, '20204Q'!A:B, 2, FALSE)</f>
+        <v>37</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>49</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <f>VLOOKUP(A41, '20204Q'!A:B, 2, FALSE)</f>
+        <v>42</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <f>VLOOKUP(A42, '20204Q'!A:B, 2, FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>35</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <f>VLOOKUP(A43, '20204Q'!A:B, 2, FALSE)</f>
+        <v>48</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="1"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>40</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <f>VLOOKUP(A44, '20204Q'!A:B, 2, FALSE)</f>
+        <v>41</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <f>VLOOKUP(A45, '20204Q'!A:B, 2, FALSE)</f>
+        <v>47</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <f>VLOOKUP(A46, '20204Q'!A:B, 2, FALSE)</f>
+        <v>43</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <f>VLOOKUP(A47, '20204Q'!A:B, 2, FALSE)</f>
+        <v>46</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>63</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <f>VLOOKUP(A48, '20204Q'!A:B, 2, FALSE)</f>
+        <v>49</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <f>VLOOKUP(A49, '20204Q'!A:B, 2, FALSE)</f>
+        <v>45</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <f>VLOOKUP(A50, '20204Q'!A:B, 2, FALSE)</f>
+        <v>44</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>45</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <f>VLOOKUP(A51, '20204Q'!A:B, 2, FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <f>VLOOKUP(A52, '20204Q'!A:B, 2, FALSE)</f>
+        <v>53</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <f>VLOOKUP(A53, '20204Q'!A:B, 2, FALSE)</f>
+        <v>56</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="1"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>55</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <f>VLOOKUP(A54, '20204Q'!A:B, 2, FALSE)</f>
+        <v>57</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="1"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>61</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <f>VLOOKUP(A55, '20204Q'!A:B, 2, FALSE)</f>
+        <v>55</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>41</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <f>VLOOKUP(A56, '20204Q'!A:B, 2, FALSE)</f>
+        <v>54</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>90</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <f>VLOOKUP(A57, '20204Q'!A:B, 2, FALSE)</f>
+        <v>59</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <f>VLOOKUP(A58, '20204Q'!A:B, 2, FALSE)</f>
+        <v>61</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="1"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59">
+        <f>VLOOKUP(A59, '20204Q'!A:B, 2, FALSE)</f>
+        <v>62</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="1"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>66</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <f>VLOOKUP(A60, '20204Q'!A:B, 2, FALSE)</f>
+        <v>51</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61">
+        <f>VLOOKUP(A61, '20204Q'!A:B, 2, FALSE)</f>
+        <v>52</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62">
+        <f>VLOOKUP(A62, '20204Q'!A:B, 2, FALSE)</f>
+        <v>69</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="1"/>
+        <v>u 8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>71</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+      <c r="C63">
+        <f>VLOOKUP(A63, '20204Q'!A:B, 2, FALSE)</f>
+        <v>60</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+      <c r="C64">
+        <f>VLOOKUP(A64, '20204Q'!A:B, 2, FALSE)</f>
+        <v>65</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>72</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65">
+        <f>VLOOKUP(A65, '20204Q'!A:B, 2, FALSE)</f>
+        <v>63</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>89</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="C66">
+        <f>VLOOKUP(A66, '20204Q'!A:B, 2, FALSE)</f>
+        <v>66</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>56</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+      <c r="C67">
+        <f>VLOOKUP(A67, '20204Q'!A:B, 2, FALSE)</f>
+        <v>58</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D101" si="2">C67-B67</f>
+        <v>-8</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" ref="E67:E101" si="3">IF(ISNA(D67), "new", IF(D67 = 0, "-", IF(D67 &gt; 0, CONCATENATE("u ", D67),   IF(D67 &lt; 0, CONCATENATE("d ", ABS(D67))))))</f>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>54</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68">
+        <f>VLOOKUP(A68, '20204Q'!A:B, 2, FALSE)</f>
+        <v>64</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="3"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69">
+        <f>VLOOKUP(A69, '20204Q'!A:B, 2, FALSE)</f>
+        <v>67</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="3"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>92</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70">
+        <f>VLOOKUP(A70, '20204Q'!A:B, 2, FALSE)</f>
+        <v>78</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="3"/>
+        <v>u 9</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>59</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71">
+        <f>VLOOKUP(A71, '20204Q'!A:B, 2, FALSE)</f>
+        <v>72</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="3"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>77</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72">
+        <f>VLOOKUP(A72, '20204Q'!A:B, 2, FALSE)</f>
+        <v>73</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="3"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>86</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+      <c r="C73">
+        <f>VLOOKUP(A73, '20204Q'!A:B, 2, FALSE)</f>
+        <v>77</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>62</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+      <c r="C74">
+        <f>VLOOKUP(A74, '20204Q'!A:B, 2, FALSE)</f>
+        <v>71</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+      <c r="C75">
+        <f>VLOOKUP(A75, '20204Q'!A:B, 2, FALSE)</f>
+        <v>68</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="2"/>
+        <v>-6</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="3"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>80</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+      <c r="C76">
+        <f>VLOOKUP(A76, '20204Q'!A:B, 2, FALSE)</f>
+        <v>89</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="3"/>
+        <v>u 14</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>69</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+      <c r="C77">
+        <f>VLOOKUP(A77, '20204Q'!A:B, 2, FALSE)</f>
+        <v>74</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>74</v>
+      </c>
+      <c r="B78">
+        <v>77</v>
+      </c>
+      <c r="C78">
+        <f>VLOOKUP(A78, '20204Q'!A:B, 2, FALSE)</f>
+        <v>70</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="2"/>
+        <v>-7</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="3"/>
+        <v>d 7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>91</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+      <c r="C79">
+        <f>VLOOKUP(A79, '20204Q'!A:B, 2, FALSE)</f>
+        <v>84</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="3"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+      <c r="C80">
+        <f>VLOOKUP(A80, '20204Q'!A:B, 2, FALSE)</f>
+        <v>80</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="3"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>70</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+      <c r="C81">
+        <f>VLOOKUP(A81, '20204Q'!A:B, 2, FALSE)</f>
+        <v>75</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="3"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>83</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+      <c r="C82">
+        <f>VLOOKUP(A82, '20204Q'!A:B, 2, FALSE)</f>
+        <v>81</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>68</v>
+      </c>
+      <c r="B83">
+        <v>82</v>
+      </c>
+      <c r="C83">
+        <f>VLOOKUP(A83, '20204Q'!A:B, 2, FALSE)</f>
+        <v>76</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="2"/>
+        <v>-6</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="3"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>103</v>
+      </c>
+      <c r="B84">
+        <v>83</v>
+      </c>
+      <c r="C84">
+        <f>VLOOKUP(A84, '20204Q'!A:B, 2, FALSE)</f>
+        <v>85</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="3"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85">
+        <v>84</v>
+      </c>
+      <c r="C85">
+        <f>VLOOKUP(A85, '20204Q'!A:B, 2, FALSE)</f>
+        <v>90</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="3"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>118</v>
+      </c>
+      <c r="B86">
+        <v>85</v>
+      </c>
+      <c r="C86" t="e">
+        <f>VLOOKUP(A86, '20204Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D86" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>88</v>
+      </c>
+      <c r="B87">
+        <v>86</v>
+      </c>
+      <c r="C87" t="e">
+        <f>VLOOKUP(A87, '20204Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D87" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>112</v>
+      </c>
+      <c r="B88">
+        <v>87</v>
+      </c>
+      <c r="C88">
+        <f>VLOOKUP(A88, '20204Q'!A:B, 2, FALSE)</f>
+        <v>95</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="3"/>
+        <v>u 8</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>75</v>
+      </c>
+      <c r="B89">
+        <v>88</v>
+      </c>
+      <c r="C89">
+        <f>VLOOKUP(A89, '20204Q'!A:B, 2, FALSE)</f>
+        <v>87</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="3"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>82</v>
+      </c>
+      <c r="B90">
+        <v>89</v>
+      </c>
+      <c r="C90">
+        <f>VLOOKUP(A90, '20204Q'!A:B, 2, FALSE)</f>
+        <v>83</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="2"/>
+        <v>-6</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="3"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>93</v>
+      </c>
+      <c r="B91">
+        <v>90</v>
+      </c>
+      <c r="C91">
+        <f>VLOOKUP(A91, '20204Q'!A:B, 2, FALSE)</f>
+        <v>82</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="3"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>100</v>
+      </c>
+      <c r="B92">
+        <v>91</v>
+      </c>
+      <c r="C92">
+        <f>VLOOKUP(A92, '20204Q'!A:B, 2, FALSE)</f>
+        <v>86</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="3"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>87</v>
+      </c>
+      <c r="B93">
+        <v>92</v>
+      </c>
+      <c r="C93">
+        <f>VLOOKUP(A93, '20204Q'!A:B, 2, FALSE)</f>
+        <v>98</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="3"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>84</v>
+      </c>
+      <c r="B94">
+        <v>93</v>
+      </c>
+      <c r="C94">
+        <f>VLOOKUP(A94, '20204Q'!A:B, 2, FALSE)</f>
+        <v>79</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="2"/>
+        <v>-14</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="3"/>
+        <v>d 14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>110</v>
+      </c>
+      <c r="B95">
+        <v>94</v>
+      </c>
+      <c r="C95">
+        <f>VLOOKUP(A95, '20204Q'!A:B, 2, FALSE)</f>
+        <v>93</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E95" t="str">
+        <f t="shared" si="3"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>119</v>
+      </c>
+      <c r="B96">
+        <v>95</v>
+      </c>
+      <c r="C96" t="e">
+        <f>VLOOKUP(A96, '20204Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D96" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>96</v>
+      </c>
+      <c r="B97">
+        <v>96</v>
+      </c>
+      <c r="C97">
+        <f>VLOOKUP(A97, '20204Q'!A:B, 2, FALSE)</f>
+        <v>91</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="3"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>114</v>
+      </c>
+      <c r="B98">
+        <v>97</v>
+      </c>
+      <c r="C98">
+        <f>VLOOKUP(A98, '20204Q'!A:B, 2, FALSE)</f>
+        <v>94</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="3"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>102</v>
+      </c>
+      <c r="B99">
+        <v>98</v>
+      </c>
+      <c r="C99">
+        <f>VLOOKUP(A99, '20204Q'!A:B, 2, FALSE)</f>
+        <v>88</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="3"/>
+        <v>d 10</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>95</v>
+      </c>
+      <c r="B100">
+        <v>99</v>
+      </c>
+      <c r="C100">
+        <f>VLOOKUP(A100, '20204Q'!A:B, 2, FALSE)</f>
+        <v>99</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>120</v>
+      </c>
+      <c r="B101">
+        <v>100</v>
+      </c>
+      <c r="C101" t="e">
+        <f>VLOOKUP(A101, '20204Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D101" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Most popular StackOverflow tags in 2Q 2021
</commit_message>
<xml_diff>
--- a/results/rank-changes.xlsx
+++ b/results/rank-changes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="20201Q" sheetId="1" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="20203Q" sheetId="3" r:id="rId3"/>
     <sheet name="20204Q" sheetId="4" r:id="rId4"/>
     <sheet name="20211Q" sheetId="5" r:id="rId5"/>
+    <sheet name="20212Q" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="123">
   <si>
     <t>Tag</t>
   </si>
@@ -394,6 +395,9 @@
   </si>
   <si>
     <t>Rank 4Q</t>
+  </si>
+  <si>
+    <t>next.js</t>
   </si>
 </sst>
 </file>
@@ -7650,8 +7654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -9682,4 +9686,2042 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>VLOOKUP(A2, '20211Q'!A:B, 2, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(ISNA(D2), "new", IF(D2 = 0, "-", IF(D2 &gt; 0, CONCATENATE("u ", D2),   IF(D2 &lt; 0, CONCATENATE("d ", ABS(D2))))))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>VLOOKUP(A3, '20211Q'!A:B, 2, FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E66" si="1">IF(ISNA(D3), "new", IF(D3 = 0, "-", IF(D3 &gt; 0, CONCATENATE("u ", D3),   IF(D3 &lt; 0, CONCATENATE("d ", ABS(D3))))))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>VLOOKUP(A4, '20211Q'!A:B, 2, FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>VLOOKUP(A5, '20211Q'!A:B, 2, FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>VLOOKUP(A6, '20211Q'!A:B, 2, FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>VLOOKUP(A7, '20211Q'!A:B, 2, FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f>VLOOKUP(A8, '20211Q'!A:B, 2, FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f>VLOOKUP(A9, '20211Q'!A:B, 2, FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f>VLOOKUP(A10, '20211Q'!A:B, 2, FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f>VLOOKUP(A11, '20211Q'!A:B, 2, FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <f>VLOOKUP(A12, '20211Q'!A:B, 2, FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f>VLOOKUP(A13, '20211Q'!A:B, 2, FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f>VLOOKUP(A14, '20211Q'!A:B, 2, FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <f>VLOOKUP(A15, '20211Q'!A:B, 2, FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <f>VLOOKUP(A16, '20211Q'!A:B, 2, FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <f>VLOOKUP(A17, '20211Q'!A:B, 2, FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f>VLOOKUP(A18, '20211Q'!A:B, 2, FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>24</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <f>VLOOKUP(A19, '20211Q'!A:B, 2, FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f>VLOOKUP(A20, '20211Q'!A:B, 2, FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <f>VLOOKUP(A21, '20211Q'!A:B, 2, FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>20</v>
+      </c>
+      <c r="C22">
+        <f>VLOOKUP(A22, '20211Q'!A:B, 2, FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f>VLOOKUP(A23, '20211Q'!A:B, 2, FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <f>VLOOKUP(A24, '20211Q'!A:B, 2, FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>34</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <f>VLOOKUP(A25, '20211Q'!A:B, 2, FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f>VLOOKUP(A26, '20211Q'!A:B, 2, FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <f>VLOOKUP(A27, '20211Q'!A:B, 2, FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>32</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <f>VLOOKUP(A28, '20211Q'!A:B, 2, FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <f>VLOOKUP(A29, '20211Q'!A:B, 2, FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <f>VLOOKUP(A30, '20211Q'!A:B, 2, FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <f>VLOOKUP(A31, '20211Q'!A:B, 2, FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <f>VLOOKUP(A32, '20211Q'!A:B, 2, FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>37</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <f>VLOOKUP(A33, '20211Q'!A:B, 2, FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>50</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <f>VLOOKUP(A34, '20211Q'!A:B, 2, FALSE)</f>
+        <v>37</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="1"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <f>VLOOKUP(A35, '20211Q'!A:B, 2, FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="1"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <f>VLOOKUP(A36, '20211Q'!A:B, 2, FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>33</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <f>VLOOKUP(A37, '20211Q'!A:B, 2, FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <f>VLOOKUP(A38, '20211Q'!A:B, 2, FALSE)</f>
+        <v>36</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <f>VLOOKUP(A39, '20211Q'!A:B, 2, FALSE)</f>
+        <v>38</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <f>VLOOKUP(A40, '20211Q'!A:B, 2, FALSE)</f>
+        <v>41</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <f>VLOOKUP(A41, '20211Q'!A:B, 2, FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>40</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <f>VLOOKUP(A42, '20211Q'!A:B, 2, FALSE)</f>
+        <v>43</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <f>VLOOKUP(A43, '20211Q'!A:B, 2, FALSE)</f>
+        <v>45</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <f>VLOOKUP(A44, '20211Q'!A:B, 2, FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <f>VLOOKUP(A45, '20211Q'!A:B, 2, FALSE)</f>
+        <v>44</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>63</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <f>VLOOKUP(A46, '20211Q'!A:B, 2, FALSE)</f>
+        <v>47</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>35</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <f>VLOOKUP(A47, '20211Q'!A:B, 2, FALSE)</f>
+        <v>42</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="1"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <f>VLOOKUP(A48, '20211Q'!A:B, 2, FALSE)</f>
+        <v>46</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <f>VLOOKUP(A49, '20211Q'!A:B, 2, FALSE)</f>
+        <v>48</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <f>VLOOKUP(A50, '20211Q'!A:B, 2, FALSE)</f>
+        <v>49</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>66</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <f>VLOOKUP(A51, '20211Q'!A:B, 2, FALSE)</f>
+        <v>59</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="1"/>
+        <v>u 9</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>60</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <f>VLOOKUP(A52, '20211Q'!A:B, 2, FALSE)</f>
+        <v>51</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <f>VLOOKUP(A53, '20211Q'!A:B, 2, FALSE)</f>
+        <v>53</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <f>VLOOKUP(A54, '20211Q'!A:B, 2, FALSE)</f>
+        <v>54</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>48</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <f>VLOOKUP(A55, '20211Q'!A:B, 2, FALSE)</f>
+        <v>52</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>90</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <f>VLOOKUP(A56, '20211Q'!A:B, 2, FALSE)</f>
+        <v>56</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>45</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <f>VLOOKUP(A57, '20211Q'!A:B, 2, FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="1"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>41</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <f>VLOOKUP(A58, '20211Q'!A:B, 2, FALSE)</f>
+        <v>55</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59">
+        <f>VLOOKUP(A59, '20211Q'!A:B, 2, FALSE)</f>
+        <v>58</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>56</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <f>VLOOKUP(A60, '20211Q'!A:B, 2, FALSE)</f>
+        <v>66</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="1"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>53</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61">
+        <f>VLOOKUP(A61, '20211Q'!A:B, 2, FALSE)</f>
+        <v>60</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>64</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62">
+        <f>VLOOKUP(A62, '20211Q'!A:B, 2, FALSE)</f>
+        <v>61</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>58</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+      <c r="C63">
+        <f>VLOOKUP(A63, '20211Q'!A:B, 2, FALSE)</f>
+        <v>57</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>65</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+      <c r="C64">
+        <f>VLOOKUP(A64, '20211Q'!A:B, 2, FALSE)</f>
+        <v>63</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>54</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65">
+        <f>VLOOKUP(A65, '20211Q'!A:B, 2, FALSE)</f>
+        <v>67</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>71</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="C66">
+        <f>VLOOKUP(A66, '20211Q'!A:B, 2, FALSE)</f>
+        <v>62</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>91</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+      <c r="C67">
+        <f>VLOOKUP(A67, '20211Q'!A:B, 2, FALSE)</f>
+        <v>78</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D101" si="2">C67-B67</f>
+        <v>12</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" ref="E67:E101" si="3">IF(ISNA(D67), "new", IF(D67 = 0, "-", IF(D67 &gt; 0, CONCATENATE("u ", D67),   IF(D67 &lt; 0, CONCATENATE("d ", ABS(D67))))))</f>
+        <v>u 12</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>72</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68">
+        <f>VLOOKUP(A68, '20211Q'!A:B, 2, FALSE)</f>
+        <v>64</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="3"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>67</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69">
+        <f>VLOOKUP(A69, '20211Q'!A:B, 2, FALSE)</f>
+        <v>68</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>86</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70">
+        <f>VLOOKUP(A70, '20211Q'!A:B, 2, FALSE)</f>
+        <v>72</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="3"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71">
+        <f>VLOOKUP(A71, '20211Q'!A:B, 2, FALSE)</f>
+        <v>73</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="3"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>73</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72">
+        <f>VLOOKUP(A72, '20211Q'!A:B, 2, FALSE)</f>
+        <v>74</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="3"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>59</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+      <c r="C73">
+        <f>VLOOKUP(A73, '20211Q'!A:B, 2, FALSE)</f>
+        <v>70</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+      <c r="C74">
+        <f>VLOOKUP(A74, '20211Q'!A:B, 2, FALSE)</f>
+        <v>75</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="3"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>104</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+      <c r="C75" t="e">
+        <f>VLOOKUP(A75, '20211Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D75" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>89</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+      <c r="C76">
+        <f>VLOOKUP(A76, '20211Q'!A:B, 2, FALSE)</f>
+        <v>65</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="3"/>
+        <v>d 10</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>74</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+      <c r="C77">
+        <f>VLOOKUP(A77, '20211Q'!A:B, 2, FALSE)</f>
+        <v>77</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="3"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>77</v>
+      </c>
+      <c r="B78">
+        <v>77</v>
+      </c>
+      <c r="C78">
+        <f>VLOOKUP(A78, '20211Q'!A:B, 2, FALSE)</f>
+        <v>71</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="2"/>
+        <v>-6</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="3"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>83</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+      <c r="C79">
+        <f>VLOOKUP(A79, '20211Q'!A:B, 2, FALSE)</f>
+        <v>81</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="3"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>79</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+      <c r="C80">
+        <f>VLOOKUP(A80, '20211Q'!A:B, 2, FALSE)</f>
+        <v>79</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>69</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+      <c r="C81">
+        <f>VLOOKUP(A81, '20211Q'!A:B, 2, FALSE)</f>
+        <v>76</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="3"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>103</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+      <c r="C82">
+        <f>VLOOKUP(A82, '20211Q'!A:B, 2, FALSE)</f>
+        <v>83</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="3"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>122</v>
+      </c>
+      <c r="B83">
+        <v>82</v>
+      </c>
+      <c r="C83" t="e">
+        <f>VLOOKUP(A83, '20211Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D83" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>70</v>
+      </c>
+      <c r="B84">
+        <v>83</v>
+      </c>
+      <c r="C84">
+        <f>VLOOKUP(A84, '20211Q'!A:B, 2, FALSE)</f>
+        <v>80</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="3"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>92</v>
+      </c>
+      <c r="B85">
+        <v>84</v>
+      </c>
+      <c r="C85">
+        <f>VLOOKUP(A85, '20211Q'!A:B, 2, FALSE)</f>
+        <v>69</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="2"/>
+        <v>-15</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="3"/>
+        <v>d 15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>82</v>
+      </c>
+      <c r="B86">
+        <v>85</v>
+      </c>
+      <c r="C86">
+        <f>VLOOKUP(A86, '20211Q'!A:B, 2, FALSE)</f>
+        <v>89</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="3"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87">
+        <v>86</v>
+      </c>
+      <c r="C87">
+        <f>VLOOKUP(A87, '20211Q'!A:B, 2, FALSE)</f>
+        <v>92</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="3"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>85</v>
+      </c>
+      <c r="B88">
+        <v>87</v>
+      </c>
+      <c r="C88">
+        <f>VLOOKUP(A88, '20211Q'!A:B, 2, FALSE)</f>
+        <v>84</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="3"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>88</v>
+      </c>
+      <c r="B89">
+        <v>88</v>
+      </c>
+      <c r="C89">
+        <f>VLOOKUP(A89, '20211Q'!A:B, 2, FALSE)</f>
+        <v>86</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>118</v>
+      </c>
+      <c r="B90">
+        <v>89</v>
+      </c>
+      <c r="C90">
+        <f>VLOOKUP(A90, '20211Q'!A:B, 2, FALSE)</f>
+        <v>85</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="3"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>112</v>
+      </c>
+      <c r="B91">
+        <v>91</v>
+      </c>
+      <c r="C91">
+        <f>VLOOKUP(A91, '20211Q'!A:B, 2, FALSE)</f>
+        <v>87</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="3"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>84</v>
+      </c>
+      <c r="B92">
+        <v>90</v>
+      </c>
+      <c r="C92">
+        <f>VLOOKUP(A92, '20211Q'!A:B, 2, FALSE)</f>
+        <v>93</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="3"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>68</v>
+      </c>
+      <c r="B93">
+        <v>92</v>
+      </c>
+      <c r="C93">
+        <f>VLOOKUP(A93, '20211Q'!A:B, 2, FALSE)</f>
+        <v>82</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="3"/>
+        <v>d 10</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>102</v>
+      </c>
+      <c r="B94">
+        <v>93</v>
+      </c>
+      <c r="C94">
+        <f>VLOOKUP(A94, '20211Q'!A:B, 2, FALSE)</f>
+        <v>98</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>95</v>
+      </c>
+      <c r="B95">
+        <v>94</v>
+      </c>
+      <c r="C95">
+        <f>VLOOKUP(A95, '20211Q'!A:B, 2, FALSE)</f>
+        <v>99</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E95" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96">
+        <v>95</v>
+      </c>
+      <c r="C96">
+        <f>VLOOKUP(A96, '20211Q'!A:B, 2, FALSE)</f>
+        <v>90</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="3"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>100</v>
+      </c>
+      <c r="B97">
+        <v>96</v>
+      </c>
+      <c r="C97">
+        <f>VLOOKUP(A97, '20211Q'!A:B, 2, FALSE)</f>
+        <v>91</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="3"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>96</v>
+      </c>
+      <c r="B98">
+        <v>97</v>
+      </c>
+      <c r="C98">
+        <f>VLOOKUP(A98, '20211Q'!A:B, 2, FALSE)</f>
+        <v>96</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="3"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>110</v>
+      </c>
+      <c r="B99">
+        <v>98</v>
+      </c>
+      <c r="C99">
+        <f>VLOOKUP(A99, '20211Q'!A:B, 2, FALSE)</f>
+        <v>94</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="3"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>116</v>
+      </c>
+      <c r="B100">
+        <v>99</v>
+      </c>
+      <c r="C100" t="e">
+        <f>VLOOKUP(A100, '20211Q'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D100" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>119</v>
+      </c>
+      <c r="B101">
+        <v>100</v>
+      </c>
+      <c r="C101">
+        <f>VLOOKUP(A101, '20211Q'!A:B, 2, FALSE)</f>
+        <v>95</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="3"/>
+        <v>d 5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Most popular StackOverflow tags in 2019
</commit_message>
<xml_diff>
--- a/results/rank-changes.xlsx
+++ b/results/rank-changes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="20201Q" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="20204Q" sheetId="4" r:id="rId4"/>
     <sheet name="20211Q" sheetId="5" r:id="rId5"/>
     <sheet name="20212Q" sheetId="6" r:id="rId6"/>
+    <sheet name="2018" sheetId="7" r:id="rId7"/>
+    <sheet name="2019" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="136">
   <si>
     <t>Tag</t>
   </si>
@@ -399,6 +401,45 @@
   <si>
     <t>next.js</t>
   </si>
+  <si>
+    <t>angularjs</t>
+  </si>
+  <si>
+    <t>python-2.7</t>
+  </si>
+  <si>
+    <t>firebase-realtime-database</t>
+  </si>
+  <si>
+    <t>maven</t>
+  </si>
+  <si>
+    <t>webpack</t>
+  </si>
+  <si>
+    <t>vb.net</t>
+  </si>
+  <si>
+    <t>ionic-framework</t>
+  </si>
+  <si>
+    <t>xamarin</t>
+  </si>
+  <si>
+    <t>laravel-5</t>
+  </si>
+  <si>
+    <t>hibernate</t>
+  </si>
+  <si>
+    <t>twitter-bootstrap</t>
+  </si>
+  <si>
+    <t>sqlite</t>
+  </si>
+  <si>
+    <t>Rank 2018</t>
+  </si>
 </sst>
 </file>
 
@@ -9692,8 +9733,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11724,4 +11765,2868 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B101"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" t="s">
+        <v>28</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29" t="s">
+        <v>24</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2">
+      <c r="A31" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32" t="s">
+        <v>40</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>49</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>38</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>59</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>62</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>39</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>33</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>43</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>34</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>123</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>56</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>67</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>76</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>77</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2">
+      <c r="A59" t="s">
+        <v>51</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2">
+      <c r="A60" t="s">
+        <v>81</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2">
+      <c r="A61" t="s">
+        <v>78</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2">
+      <c r="A62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2">
+      <c r="A63" t="s">
+        <v>57</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2">
+      <c r="A64" t="s">
+        <v>61</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2">
+      <c r="A65" t="s">
+        <v>66</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2">
+      <c r="A66" t="s">
+        <v>64</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
+      <c r="A67" t="s">
+        <v>124</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2">
+      <c r="A68" t="s">
+        <v>44</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2">
+      <c r="A69" t="s">
+        <v>60</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
+      <c r="A70" t="s">
+        <v>79</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2">
+      <c r="A71" t="s">
+        <v>98</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2">
+      <c r="A72" t="s">
+        <v>45</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2">
+      <c r="A73" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2">
+      <c r="A74" t="s">
+        <v>63</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2">
+      <c r="A75" t="s">
+        <v>96</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2">
+      <c r="A76" t="s">
+        <v>71</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2">
+      <c r="A77" t="s">
+        <v>95</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2">
+      <c r="A78" t="s">
+        <v>94</v>
+      </c>
+      <c r="B78">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2">
+      <c r="A79" t="s">
+        <v>73</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2">
+      <c r="A80" t="s">
+        <v>87</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2">
+      <c r="A81" t="s">
+        <v>125</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2">
+      <c r="A82" t="s">
+        <v>84</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2">
+      <c r="A84" t="s">
+        <v>92</v>
+      </c>
+      <c r="B84">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2">
+      <c r="A85" t="s">
+        <v>126</v>
+      </c>
+      <c r="B85">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2">
+      <c r="A86" t="s">
+        <v>97</v>
+      </c>
+      <c r="B86">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2">
+      <c r="A87" t="s">
+        <v>27</v>
+      </c>
+      <c r="B87">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2">
+      <c r="A88" t="s">
+        <v>72</v>
+      </c>
+      <c r="B88">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2">
+      <c r="A89" t="s">
+        <v>75</v>
+      </c>
+      <c r="B89">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2">
+      <c r="A90" t="s">
+        <v>127</v>
+      </c>
+      <c r="B90">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2">
+      <c r="A91" t="s">
+        <v>128</v>
+      </c>
+      <c r="B91">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2">
+      <c r="A92" t="s">
+        <v>129</v>
+      </c>
+      <c r="B92">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2">
+      <c r="A93" t="s">
+        <v>65</v>
+      </c>
+      <c r="B93">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2">
+      <c r="A94" t="s">
+        <v>130</v>
+      </c>
+      <c r="B94">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2">
+      <c r="A95" t="s">
+        <v>131</v>
+      </c>
+      <c r="B95">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2">
+      <c r="A96" t="s">
+        <v>83</v>
+      </c>
+      <c r="B96">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2">
+      <c r="A97" t="s">
+        <v>74</v>
+      </c>
+      <c r="B97">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2">
+      <c r="A98" t="s">
+        <v>132</v>
+      </c>
+      <c r="B98">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2">
+      <c r="A99" t="s">
+        <v>133</v>
+      </c>
+      <c r="B99">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2">
+      <c r="A100" t="s">
+        <v>101</v>
+      </c>
+      <c r="B100">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2">
+      <c r="A101" t="s">
+        <v>134</v>
+      </c>
+      <c r="B101">
+        <v>100</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E101"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>VLOOKUP(A2, '2018'!A:B, 2, FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(ISNA(D2), "new", IF(D2 = 0, "-", IF(D2 &gt; 0, CONCATENATE("u ", D2),   IF(D2 &lt; 0, CONCATENATE("d ", ABS(D2))))))</f>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>VLOOKUP(A3, '2018'!A:B, 2, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">C3-B3</f>
+        <v>-1</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E66" si="1">IF(ISNA(D3), "new", IF(D3 = 0, "-", IF(D3 &gt; 0, CONCATENATE("u ", D3),   IF(D3 &lt; 0, CONCATENATE("d ", ABS(D3))))))</f>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>VLOOKUP(A4, '2018'!A:B, 2, FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>VLOOKUP(A5, '2018'!A:B, 2, FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>VLOOKUP(A6, '2018'!A:B, 2, FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>VLOOKUP(A7, '2018'!A:B, 2, FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f>VLOOKUP(A8, '2018'!A:B, 2, FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f>VLOOKUP(A9, '2018'!A:B, 2, FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f>VLOOKUP(A10, '2018'!A:B, 2, FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>u 8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f>VLOOKUP(A11, '2018'!A:B, 2, FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <f>VLOOKUP(A12, '2018'!A:B, 2, FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f>VLOOKUP(A13, '2018'!A:B, 2, FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f>VLOOKUP(A14, '2018'!A:B, 2, FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <f>VLOOKUP(A15, '2018'!A:B, 2, FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <f>VLOOKUP(A16, '2018'!A:B, 2, FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <f>VLOOKUP(A17, '2018'!A:B, 2, FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f>VLOOKUP(A18, '2018'!A:B, 2, FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <f>VLOOKUP(A19, '2018'!A:B, 2, FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f>VLOOKUP(A20, '2018'!A:B, 2, FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f>VLOOKUP(A21, '2018'!A:B, 2, FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <f>VLOOKUP(A22, '2018'!A:B, 2, FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f>VLOOKUP(A23, '2018'!A:B, 2, FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <f>VLOOKUP(A24, '2018'!A:B, 2, FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <f>VLOOKUP(A25, '2018'!A:B, 2, FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f>VLOOKUP(A26, '2018'!A:B, 2, FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <f>VLOOKUP(A27, '2018'!A:B, 2, FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <f>VLOOKUP(A28, '2018'!A:B, 2, FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <f>VLOOKUP(A29, '2018'!A:B, 2, FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <f>VLOOKUP(A30, '2018'!A:B, 2, FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <f>VLOOKUP(A31, '2018'!A:B, 2, FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <f>VLOOKUP(A32, '2018'!A:B, 2, FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <f>VLOOKUP(A33, '2018'!A:B, 2, FALSE)</f>
+        <v>86</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>u 54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <f>VLOOKUP(A34, '2018'!A:B, 2, FALSE)</f>
+        <v>45</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="1"/>
+        <v>u 12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <f>VLOOKUP(A35, '2018'!A:B, 2, FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <f>VLOOKUP(A36, '2018'!A:B, 2, FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <f>VLOOKUP(A37, '2018'!A:B, 2, FALSE)</f>
+        <v>38</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <f>VLOOKUP(A38, '2018'!A:B, 2, FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="1"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <f>VLOOKUP(A39, '2018'!A:B, 2, FALSE)</f>
+        <v>36</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <f>VLOOKUP(A40, '2018'!A:B, 2, FALSE)</f>
+        <v>49</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="1"/>
+        <v>u 10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <f>VLOOKUP(A41, '2018'!A:B, 2, FALSE)</f>
+        <v>42</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <f>VLOOKUP(A42, '2018'!A:B, 2, FALSE)</f>
+        <v>48</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="1"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <f>VLOOKUP(A43, '2018'!A:B, 2, FALSE)</f>
+        <v>41</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <f>VLOOKUP(A44, '2018'!A:B, 2, FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <f>VLOOKUP(A45, '2018'!A:B, 2, FALSE)</f>
+        <v>67</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="1"/>
+        <v>u 23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <f>VLOOKUP(A46, '2018'!A:B, 2, FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <f>VLOOKUP(A47, '2018'!A:B, 2, FALSE)</f>
+        <v>46</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <f>VLOOKUP(A48, '2018'!A:B, 2, FALSE)</f>
+        <v>71</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="1"/>
+        <v>u 24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <f>VLOOKUP(A49, '2018'!A:B, 2, FALSE)</f>
+        <v>37</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>-11</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="1"/>
+        <v>d 11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <f>VLOOKUP(A50, '2018'!A:B, 2, FALSE)</f>
+        <v>58</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="1"/>
+        <v>u 9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <f>VLOOKUP(A51, '2018'!A:B, 2, FALSE)</f>
+        <v>51</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <f>VLOOKUP(A52, '2018'!A:B, 2, FALSE)</f>
+        <v>52</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <f>VLOOKUP(A53, '2018'!A:B, 2, FALSE)</f>
+        <v>44</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <f>VLOOKUP(A54, '2018'!A:B, 2, FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>-14</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="1"/>
+        <v>d 14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <f>VLOOKUP(A55, '2018'!A:B, 2, FALSE)</f>
+        <v>62</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="1"/>
+        <v>u 8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <f>VLOOKUP(A56, '2018'!A:B, 2, FALSE)</f>
+        <v>53</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <f>VLOOKUP(A57, '2018'!A:B, 2, FALSE)</f>
+        <v>61</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="1"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <f>VLOOKUP(A58, '2018'!A:B, 2, FALSE)</f>
+        <v>47</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="1"/>
+        <v>d 10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59">
+        <f>VLOOKUP(A59, '2018'!A:B, 2, FALSE)</f>
+        <v>55</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <f>VLOOKUP(A60, '2018'!A:B, 2, FALSE)</f>
+        <v>43</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>-16</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="1"/>
+        <v>d 16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61" t="e">
+        <f>VLOOKUP(A61, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D61" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="1"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62">
+        <f>VLOOKUP(A62, '2018'!A:B, 2, FALSE)</f>
+        <v>63</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+      <c r="C63">
+        <f>VLOOKUP(A63, '2018'!A:B, 2, FALSE)</f>
+        <v>54</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+      <c r="C64">
+        <f>VLOOKUP(A64, '2018'!A:B, 2, FALSE)</f>
+        <v>68</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="1"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65">
+        <f>VLOOKUP(A65, '2018'!A:B, 2, FALSE)</f>
+        <v>65</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="C66">
+        <f>VLOOKUP(A66, '2018'!A:B, 2, FALSE)</f>
+        <v>57</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+      <c r="C67">
+        <f>VLOOKUP(A67, '2018'!A:B, 2, FALSE)</f>
+        <v>92</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D101" si="2">C67-B67</f>
+        <v>26</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" ref="E67:E101" si="3">IF(ISNA(D67), "new", IF(D67 = 0, "-", IF(D67 &gt; 0, CONCATENATE("u ", D67),   IF(D67 &lt; 0, CONCATENATE("d ", ABS(D67))))))</f>
+        <v>u 26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68">
+        <f>VLOOKUP(A68, '2018'!A:B, 2, FALSE)</f>
+        <v>56</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="2"/>
+        <v>-11</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="3"/>
+        <v>d 11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>78</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69">
+        <f>VLOOKUP(A69, '2018'!A:B, 2, FALSE)</f>
+        <v>60</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="3"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70">
+        <f>VLOOKUP(A70, '2018'!A:B, 2, FALSE)</f>
+        <v>76</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="3"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71">
+        <f>VLOOKUP(A71, '2018'!A:B, 2, FALSE)</f>
+        <v>73</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="3"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>81</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72">
+        <f>VLOOKUP(A72, '2018'!A:B, 2, FALSE)</f>
+        <v>59</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="2"/>
+        <v>-12</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="3"/>
+        <v>d 12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+      <c r="C73">
+        <f>VLOOKUP(A73, '2018'!A:B, 2, FALSE)</f>
+        <v>96</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="3"/>
+        <v>u 24</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>71</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+      <c r="C74">
+        <f>VLOOKUP(A74, '2018'!A:B, 2, FALSE)</f>
+        <v>75</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="3"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>69</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+      <c r="C75">
+        <f>VLOOKUP(A75, '2018'!A:B, 2, FALSE)</f>
+        <v>72</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+      <c r="C76" t="e">
+        <f>VLOOKUP(A76, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D76" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>73</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+      <c r="C77">
+        <f>VLOOKUP(A77, '2018'!A:B, 2, FALSE)</f>
+        <v>78</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="3"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78">
+        <v>77</v>
+      </c>
+      <c r="C78">
+        <f>VLOOKUP(A78, '2018'!A:B, 2, FALSE)</f>
+        <v>69</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="3"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>72</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+      <c r="C79">
+        <f>VLOOKUP(A79, '2018'!A:B, 2, FALSE)</f>
+        <v>87</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="3"/>
+        <v>u 9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>98</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+      <c r="C80">
+        <f>VLOOKUP(A80, '2018'!A:B, 2, FALSE)</f>
+        <v>70</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="3"/>
+        <v>d 9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>87</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+      <c r="C81">
+        <f>VLOOKUP(A81, '2018'!A:B, 2, FALSE)</f>
+        <v>79</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="3"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+      <c r="C82">
+        <f>VLOOKUP(A82, '2018'!A:B, 2, FALSE)</f>
+        <v>64</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="2"/>
+        <v>-17</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="3"/>
+        <v>d 17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>82</v>
+      </c>
+      <c r="C83">
+        <f>VLOOKUP(A83, '2018'!A:B, 2, FALSE)</f>
+        <v>82</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84">
+        <v>83</v>
+      </c>
+      <c r="C84">
+        <f>VLOOKUP(A84, '2018'!A:B, 2, FALSE)</f>
+        <v>81</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>75</v>
+      </c>
+      <c r="B85">
+        <v>84</v>
+      </c>
+      <c r="C85">
+        <f>VLOOKUP(A85, '2018'!A:B, 2, FALSE)</f>
+        <v>88</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="3"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>96</v>
+      </c>
+      <c r="B86">
+        <v>85</v>
+      </c>
+      <c r="C86">
+        <f>VLOOKUP(A86, '2018'!A:B, 2, FALSE)</f>
+        <v>74</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="2"/>
+        <v>-11</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="3"/>
+        <v>d 11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>94</v>
+      </c>
+      <c r="B87">
+        <v>86</v>
+      </c>
+      <c r="C87">
+        <f>VLOOKUP(A87, '2018'!A:B, 2, FALSE)</f>
+        <v>77</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="3"/>
+        <v>d 9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>92</v>
+      </c>
+      <c r="B88">
+        <v>87</v>
+      </c>
+      <c r="C88">
+        <f>VLOOKUP(A88, '2018'!A:B, 2, FALSE)</f>
+        <v>83</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="3"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89">
+        <v>88</v>
+      </c>
+      <c r="C89" t="e">
+        <f>VLOOKUP(A89, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D89" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>83</v>
+      </c>
+      <c r="B90">
+        <v>89</v>
+      </c>
+      <c r="C90">
+        <f>VLOOKUP(A90, '2018'!A:B, 2, FALSE)</f>
+        <v>95</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="3"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>86</v>
+      </c>
+      <c r="B91">
+        <v>90</v>
+      </c>
+      <c r="C91" t="e">
+        <f>VLOOKUP(A91, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D91" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>80</v>
+      </c>
+      <c r="B92">
+        <v>91</v>
+      </c>
+      <c r="C92" t="e">
+        <f>VLOOKUP(A92, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D92" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>88</v>
+      </c>
+      <c r="B93">
+        <v>92</v>
+      </c>
+      <c r="C93" t="e">
+        <f>VLOOKUP(A93, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D93" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>128</v>
+      </c>
+      <c r="B94">
+        <v>93</v>
+      </c>
+      <c r="C94">
+        <f>VLOOKUP(A94, '2018'!A:B, 2, FALSE)</f>
+        <v>90</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="3"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>90</v>
+      </c>
+      <c r="B95">
+        <v>94</v>
+      </c>
+      <c r="C95" t="e">
+        <f>VLOOKUP(A95, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D95" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E95" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>91</v>
+      </c>
+      <c r="B96">
+        <v>95</v>
+      </c>
+      <c r="C96" t="e">
+        <f>VLOOKUP(A96, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D96" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>99</v>
+      </c>
+      <c r="B97">
+        <v>96</v>
+      </c>
+      <c r="C97" t="e">
+        <f>VLOOKUP(A97, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D97" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>97</v>
+      </c>
+      <c r="C98">
+        <f>VLOOKUP(A98, '2018'!A:B, 2, FALSE)</f>
+        <v>85</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="2"/>
+        <v>-12</v>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="3"/>
+        <v>d 12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>106</v>
+      </c>
+      <c r="B99">
+        <v>98</v>
+      </c>
+      <c r="C99" t="e">
+        <f>VLOOKUP(A99, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D99" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>116</v>
+      </c>
+      <c r="B100">
+        <v>99</v>
+      </c>
+      <c r="C100" t="e">
+        <f>VLOOKUP(A100, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D100" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>126</v>
+      </c>
+      <c r="B101">
+        <v>100</v>
+      </c>
+      <c r="C101">
+        <f>VLOOKUP(A101, '2018'!A:B, 2, FALSE)</f>
+        <v>84</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="2"/>
+        <v>-16</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="3"/>
+        <v>d 16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Add Most popular StackOverflow tags in 2020
</commit_message>
<xml_diff>
--- a/results/rank-changes.xlsx
+++ b/results/rank-changes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="20201Q" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="20212Q" sheetId="6" r:id="rId6"/>
     <sheet name="2018" sheetId="7" r:id="rId7"/>
     <sheet name="2019" sheetId="8" r:id="rId8"/>
+    <sheet name="2020" sheetId="9" r:id="rId9"/>
+    <sheet name="2021" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="834" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="137">
   <si>
     <t>Tag</t>
   </si>
@@ -440,6 +442,9 @@
   <si>
     <t>Rank 2018</t>
   </si>
+  <si>
+    <t>Rank 2019</t>
+  </si>
 </sst>
 </file>
 
@@ -1581,6 +1586,18 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
@@ -12598,6 +12615,2043 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>VLOOKUP(A2, '2018'!A:B, 2, FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>1</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(ISNA(D2), "new", IF(D2 = 0, "-", IF(D2 &gt; 0, CONCATENATE("u ", D2),   IF(D2 &lt; 0, CONCATENATE("d ", ABS(D2))))))</f>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>VLOOKUP(A3, '2018'!A:B, 2, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">C3-B3</f>
+        <v>-1</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E66" si="1">IF(ISNA(D3), "new", IF(D3 = 0, "-", IF(D3 &gt; 0, CONCATENATE("u ", D3),   IF(D3 &lt; 0, CONCATENATE("d ", ABS(D3))))))</f>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>VLOOKUP(A4, '2018'!A:B, 2, FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>VLOOKUP(A5, '2018'!A:B, 2, FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>VLOOKUP(A6, '2018'!A:B, 2, FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>VLOOKUP(A7, '2018'!A:B, 2, FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f>VLOOKUP(A8, '2018'!A:B, 2, FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f>VLOOKUP(A9, '2018'!A:B, 2, FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f>VLOOKUP(A10, '2018'!A:B, 2, FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>u 8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f>VLOOKUP(A11, '2018'!A:B, 2, FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <f>VLOOKUP(A12, '2018'!A:B, 2, FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>15</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f>VLOOKUP(A13, '2018'!A:B, 2, FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f>VLOOKUP(A14, '2018'!A:B, 2, FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <f>VLOOKUP(A15, '2018'!A:B, 2, FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <f>VLOOKUP(A16, '2018'!A:B, 2, FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <f>VLOOKUP(A17, '2018'!A:B, 2, FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f>VLOOKUP(A18, '2018'!A:B, 2, FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <f>VLOOKUP(A19, '2018'!A:B, 2, FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f>VLOOKUP(A20, '2018'!A:B, 2, FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>22</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f>VLOOKUP(A21, '2018'!A:B, 2, FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <f>VLOOKUP(A22, '2018'!A:B, 2, FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f>VLOOKUP(A23, '2018'!A:B, 2, FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <f>VLOOKUP(A24, '2018'!A:B, 2, FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <f>VLOOKUP(A25, '2018'!A:B, 2, FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f>VLOOKUP(A26, '2018'!A:B, 2, FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <f>VLOOKUP(A27, '2018'!A:B, 2, FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <f>VLOOKUP(A28, '2018'!A:B, 2, FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <f>VLOOKUP(A29, '2018'!A:B, 2, FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <f>VLOOKUP(A30, '2018'!A:B, 2, FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <f>VLOOKUP(A31, '2018'!A:B, 2, FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <f>VLOOKUP(A32, '2018'!A:B, 2, FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <f>VLOOKUP(A33, '2018'!A:B, 2, FALSE)</f>
+        <v>86</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>u 54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <f>VLOOKUP(A34, '2018'!A:B, 2, FALSE)</f>
+        <v>45</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="1"/>
+        <v>u 12</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>41</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <f>VLOOKUP(A35, '2018'!A:B, 2, FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>37</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <f>VLOOKUP(A36, '2018'!A:B, 2, FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <f>VLOOKUP(A37, '2018'!A:B, 2, FALSE)</f>
+        <v>38</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <f>VLOOKUP(A38, '2018'!A:B, 2, FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="1"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <f>VLOOKUP(A39, '2018'!A:B, 2, FALSE)</f>
+        <v>36</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>34</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <f>VLOOKUP(A40, '2018'!A:B, 2, FALSE)</f>
+        <v>49</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="1"/>
+        <v>u 10</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>39</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <f>VLOOKUP(A41, '2018'!A:B, 2, FALSE)</f>
+        <v>42</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>43</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <f>VLOOKUP(A42, '2018'!A:B, 2, FALSE)</f>
+        <v>48</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="1"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <f>VLOOKUP(A43, '2018'!A:B, 2, FALSE)</f>
+        <v>41</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>49</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <f>VLOOKUP(A44, '2018'!A:B, 2, FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <f>VLOOKUP(A45, '2018'!A:B, 2, FALSE)</f>
+        <v>67</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="1"/>
+        <v>u 23</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <f>VLOOKUP(A46, '2018'!A:B, 2, FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>52</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <f>VLOOKUP(A47, '2018'!A:B, 2, FALSE)</f>
+        <v>46</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <f>VLOOKUP(A48, '2018'!A:B, 2, FALSE)</f>
+        <v>71</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="1"/>
+        <v>u 24</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>59</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <f>VLOOKUP(A49, '2018'!A:B, 2, FALSE)</f>
+        <v>37</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>-11</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="1"/>
+        <v>d 11</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>51</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <f>VLOOKUP(A50, '2018'!A:B, 2, FALSE)</f>
+        <v>58</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="1"/>
+        <v>u 9</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>54</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <f>VLOOKUP(A51, '2018'!A:B, 2, FALSE)</f>
+        <v>51</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <f>VLOOKUP(A52, '2018'!A:B, 2, FALSE)</f>
+        <v>52</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>46</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <f>VLOOKUP(A53, '2018'!A:B, 2, FALSE)</f>
+        <v>44</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>62</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <f>VLOOKUP(A54, '2018'!A:B, 2, FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>-14</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="1"/>
+        <v>d 14</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <f>VLOOKUP(A55, '2018'!A:B, 2, FALSE)</f>
+        <v>62</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="1"/>
+        <v>u 8</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <f>VLOOKUP(A56, '2018'!A:B, 2, FALSE)</f>
+        <v>53</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>47</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <f>VLOOKUP(A57, '2018'!A:B, 2, FALSE)</f>
+        <v>61</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="1"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <f>VLOOKUP(A58, '2018'!A:B, 2, FALSE)</f>
+        <v>47</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="1"/>
+        <v>d 10</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59">
+        <f>VLOOKUP(A59, '2018'!A:B, 2, FALSE)</f>
+        <v>55</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>70</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <f>VLOOKUP(A60, '2018'!A:B, 2, FALSE)</f>
+        <v>43</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>-16</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="1"/>
+        <v>d 16</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61" t="e">
+        <f>VLOOKUP(A61, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D61" t="e">
+        <f t="shared" si="0"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="1"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62">
+        <f>VLOOKUP(A62, '2018'!A:B, 2, FALSE)</f>
+        <v>63</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>67</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+      <c r="C63">
+        <f>VLOOKUP(A63, '2018'!A:B, 2, FALSE)</f>
+        <v>54</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>60</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+      <c r="C64">
+        <f>VLOOKUP(A64, '2018'!A:B, 2, FALSE)</f>
+        <v>68</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="1"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65">
+        <f>VLOOKUP(A65, '2018'!A:B, 2, FALSE)</f>
+        <v>65</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>77</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="C66">
+        <f>VLOOKUP(A66, '2018'!A:B, 2, FALSE)</f>
+        <v>57</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>65</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+      <c r="C67">
+        <f>VLOOKUP(A67, '2018'!A:B, 2, FALSE)</f>
+        <v>92</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D101" si="2">C67-B67</f>
+        <v>26</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" ref="E67:E101" si="3">IF(ISNA(D67), "new", IF(D67 = 0, "-", IF(D67 &gt; 0, CONCATENATE("u ", D67),   IF(D67 &lt; 0, CONCATENATE("d ", ABS(D67))))))</f>
+        <v>u 26</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>76</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68">
+        <f>VLOOKUP(A68, '2018'!A:B, 2, FALSE)</f>
+        <v>56</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="2"/>
+        <v>-11</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="3"/>
+        <v>d 11</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>78</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69">
+        <f>VLOOKUP(A69, '2018'!A:B, 2, FALSE)</f>
+        <v>60</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="3"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70">
+        <f>VLOOKUP(A70, '2018'!A:B, 2, FALSE)</f>
+        <v>76</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="3"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>63</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71">
+        <f>VLOOKUP(A71, '2018'!A:B, 2, FALSE)</f>
+        <v>73</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="3"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>81</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72">
+        <f>VLOOKUP(A72, '2018'!A:B, 2, FALSE)</f>
+        <v>59</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="2"/>
+        <v>-12</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="3"/>
+        <v>d 12</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>74</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+      <c r="C73">
+        <f>VLOOKUP(A73, '2018'!A:B, 2, FALSE)</f>
+        <v>96</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="2"/>
+        <v>24</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="3"/>
+        <v>u 24</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>71</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+      <c r="C74">
+        <f>VLOOKUP(A74, '2018'!A:B, 2, FALSE)</f>
+        <v>75</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="3"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>69</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+      <c r="C75">
+        <f>VLOOKUP(A75, '2018'!A:B, 2, FALSE)</f>
+        <v>72</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>68</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+      <c r="C76" t="e">
+        <f>VLOOKUP(A76, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D76" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>73</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+      <c r="C77">
+        <f>VLOOKUP(A77, '2018'!A:B, 2, FALSE)</f>
+        <v>78</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="3"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78">
+        <v>77</v>
+      </c>
+      <c r="C78">
+        <f>VLOOKUP(A78, '2018'!A:B, 2, FALSE)</f>
+        <v>69</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="3"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>72</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+      <c r="C79">
+        <f>VLOOKUP(A79, '2018'!A:B, 2, FALSE)</f>
+        <v>87</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="2"/>
+        <v>9</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="3"/>
+        <v>u 9</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>98</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+      <c r="C80">
+        <f>VLOOKUP(A80, '2018'!A:B, 2, FALSE)</f>
+        <v>70</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="3"/>
+        <v>d 9</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>87</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+      <c r="C81">
+        <f>VLOOKUP(A81, '2018'!A:B, 2, FALSE)</f>
+        <v>79</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="3"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>66</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+      <c r="C82">
+        <f>VLOOKUP(A82, '2018'!A:B, 2, FALSE)</f>
+        <v>64</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="2"/>
+        <v>-17</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="3"/>
+        <v>d 17</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>82</v>
+      </c>
+      <c r="B83">
+        <v>82</v>
+      </c>
+      <c r="C83">
+        <f>VLOOKUP(A83, '2018'!A:B, 2, FALSE)</f>
+        <v>82</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84">
+        <v>83</v>
+      </c>
+      <c r="C84">
+        <f>VLOOKUP(A84, '2018'!A:B, 2, FALSE)</f>
+        <v>81</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>75</v>
+      </c>
+      <c r="B85">
+        <v>84</v>
+      </c>
+      <c r="C85">
+        <f>VLOOKUP(A85, '2018'!A:B, 2, FALSE)</f>
+        <v>88</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="3"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>96</v>
+      </c>
+      <c r="B86">
+        <v>85</v>
+      </c>
+      <c r="C86">
+        <f>VLOOKUP(A86, '2018'!A:B, 2, FALSE)</f>
+        <v>74</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="2"/>
+        <v>-11</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="3"/>
+        <v>d 11</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>94</v>
+      </c>
+      <c r="B87">
+        <v>86</v>
+      </c>
+      <c r="C87">
+        <f>VLOOKUP(A87, '2018'!A:B, 2, FALSE)</f>
+        <v>77</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="3"/>
+        <v>d 9</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>92</v>
+      </c>
+      <c r="B88">
+        <v>87</v>
+      </c>
+      <c r="C88">
+        <f>VLOOKUP(A88, '2018'!A:B, 2, FALSE)</f>
+        <v>83</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="3"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>85</v>
+      </c>
+      <c r="B89">
+        <v>88</v>
+      </c>
+      <c r="C89" t="e">
+        <f>VLOOKUP(A89, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D89" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>83</v>
+      </c>
+      <c r="B90">
+        <v>89</v>
+      </c>
+      <c r="C90">
+        <f>VLOOKUP(A90, '2018'!A:B, 2, FALSE)</f>
+        <v>95</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="3"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>86</v>
+      </c>
+      <c r="B91">
+        <v>90</v>
+      </c>
+      <c r="C91" t="e">
+        <f>VLOOKUP(A91, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D91" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>80</v>
+      </c>
+      <c r="B92">
+        <v>91</v>
+      </c>
+      <c r="C92" t="e">
+        <f>VLOOKUP(A92, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D92" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>88</v>
+      </c>
+      <c r="B93">
+        <v>92</v>
+      </c>
+      <c r="C93" t="e">
+        <f>VLOOKUP(A93, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D93" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>128</v>
+      </c>
+      <c r="B94">
+        <v>93</v>
+      </c>
+      <c r="C94">
+        <f>VLOOKUP(A94, '2018'!A:B, 2, FALSE)</f>
+        <v>90</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="3"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>90</v>
+      </c>
+      <c r="B95">
+        <v>94</v>
+      </c>
+      <c r="C95" t="e">
+        <f>VLOOKUP(A95, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D95" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E95" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>91</v>
+      </c>
+      <c r="B96">
+        <v>95</v>
+      </c>
+      <c r="C96" t="e">
+        <f>VLOOKUP(A96, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D96" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>99</v>
+      </c>
+      <c r="B97">
+        <v>96</v>
+      </c>
+      <c r="C97" t="e">
+        <f>VLOOKUP(A97, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D97" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>97</v>
+      </c>
+      <c r="B98">
+        <v>97</v>
+      </c>
+      <c r="C98">
+        <f>VLOOKUP(A98, '2018'!A:B, 2, FALSE)</f>
+        <v>85</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="2"/>
+        <v>-12</v>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="3"/>
+        <v>d 12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>106</v>
+      </c>
+      <c r="B99">
+        <v>98</v>
+      </c>
+      <c r="C99" t="e">
+        <f>VLOOKUP(A99, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D99" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>116</v>
+      </c>
+      <c r="B100">
+        <v>99</v>
+      </c>
+      <c r="C100" t="e">
+        <f>VLOOKUP(A100, '2018'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D100" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>126</v>
+      </c>
+      <c r="B101">
+        <v>100</v>
+      </c>
+      <c r="C101">
+        <f>VLOOKUP(A101, '2018'!A:B, 2, FALSE)</f>
+        <v>84</v>
+      </c>
+      <c r="D101">
+        <f t="shared" si="2"/>
+        <v>-16</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="3"/>
+        <v>d 16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E101"/>
+  <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
@@ -12617,7 +14671,7 @@
         <v>109</v>
       </c>
       <c r="C1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="D1" t="s">
         <v>108</v>
@@ -12634,16 +14688,16 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <f>VLOOKUP(A2, '2018'!A:B, 2, FALSE)</f>
-        <v>2</v>
+        <f>VLOOKUP(A2, '2019'!A:B, 2, FALSE)</f>
+        <v>1</v>
       </c>
       <c r="D2">
         <f>C2-B2</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="str">
         <f>IF(ISNA(D2), "new", IF(D2 = 0, "-", IF(D2 &gt; 0, CONCATENATE("u ", D2),   IF(D2 &lt; 0, CONCATENATE("d ", ABS(D2))))))</f>
-        <v>u 1</v>
+        <v>-</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -12654,16 +14708,16 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <f>VLOOKUP(A3, '2018'!A:B, 2, FALSE)</f>
-        <v>1</v>
+        <f>VLOOKUP(A3, '2019'!A:B, 2, FALSE)</f>
+        <v>2</v>
       </c>
       <c r="D3">
         <f t="shared" ref="D3:D66" si="0">C3-B3</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="str">
         <f t="shared" ref="E3:E66" si="1">IF(ISNA(D3), "new", IF(D3 = 0, "-", IF(D3 &gt; 0, CONCATENATE("u ", D3),   IF(D3 &lt; 0, CONCATENATE("d ", ABS(D3))))))</f>
-        <v>d 1</v>
+        <v>-</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -12674,7 +14728,7 @@
         <v>3</v>
       </c>
       <c r="C4">
-        <f>VLOOKUP(A4, '2018'!A:B, 2, FALSE)</f>
+        <f>VLOOKUP(A4, '2019'!A:B, 2, FALSE)</f>
         <v>3</v>
       </c>
       <c r="D4">
@@ -12694,7 +14748,7 @@
         <v>4</v>
       </c>
       <c r="C5">
-        <f>VLOOKUP(A5, '2018'!A:B, 2, FALSE)</f>
+        <f>VLOOKUP(A5, '2019'!A:B, 2, FALSE)</f>
         <v>4</v>
       </c>
       <c r="D5">
@@ -12708,193 +14762,193 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6">
-        <f>VLOOKUP(A6, '2018'!A:B, 2, FALSE)</f>
-        <v>5</v>
+        <f>VLOOKUP(A6, '2019'!A:B, 2, FALSE)</f>
+        <v>9</v>
       </c>
       <c r="D6">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E6" t="str">
         <f t="shared" si="1"/>
-        <v>-</v>
+        <v>u 4</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7">
-        <f>VLOOKUP(A7, '2018'!A:B, 2, FALSE)</f>
-        <v>6</v>
+        <f>VLOOKUP(A7, '2019'!A:B, 2, FALSE)</f>
+        <v>7</v>
       </c>
       <c r="D7">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="str">
         <f t="shared" si="1"/>
-        <v>-</v>
+        <v>u 1</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8">
-        <f>VLOOKUP(A8, '2018'!A:B, 2, FALSE)</f>
-        <v>7</v>
+        <f>VLOOKUP(A8, '2019'!A:B, 2, FALSE)</f>
+        <v>5</v>
       </c>
       <c r="D8">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="E8" t="str">
         <f t="shared" si="1"/>
-        <v>-</v>
+        <v>d 2</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9">
-        <f>VLOOKUP(A9, '2018'!A:B, 2, FALSE)</f>
-        <v>14</v>
+        <f>VLOOKUP(A9, '2019'!A:B, 2, FALSE)</f>
+        <v>6</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-2</v>
       </c>
       <c r="E9" t="str">
         <f t="shared" si="1"/>
-        <v>u 6</v>
+        <v>d 2</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10">
-        <f>VLOOKUP(A10, '2018'!A:B, 2, FALSE)</f>
-        <v>17</v>
+        <f>VLOOKUP(A10, '2019'!A:B, 2, FALSE)</f>
+        <v>8</v>
       </c>
       <c r="D10">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>-1</v>
       </c>
       <c r="E10" t="str">
         <f t="shared" si="1"/>
-        <v>u 8</v>
+        <v>d 1</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11">
-        <f>VLOOKUP(A11, '2018'!A:B, 2, FALSE)</f>
-        <v>9</v>
+        <f>VLOOKUP(A11, '2019'!A:B, 2, FALSE)</f>
+        <v>11</v>
       </c>
       <c r="D11">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E11" t="str">
         <f t="shared" si="1"/>
-        <v>d 1</v>
+        <v>u 1</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12">
-        <f>VLOOKUP(A12, '2018'!A:B, 2, FALSE)</f>
-        <v>12</v>
+        <f>VLOOKUP(A12, '2019'!A:B, 2, FALSE)</f>
+        <v>15</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E12" t="str">
         <f t="shared" si="1"/>
-        <v>u 1</v>
+        <v>u 4</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13">
-        <f>VLOOKUP(A13, '2018'!A:B, 2, FALSE)</f>
-        <v>8</v>
+        <f>VLOOKUP(A13, '2019'!A:B, 2, FALSE)</f>
+        <v>14</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>-4</v>
+        <v>2</v>
       </c>
       <c r="E13" t="str">
         <f t="shared" si="1"/>
-        <v>d 4</v>
+        <v>u 2</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14">
-        <f>VLOOKUP(A14, '2018'!A:B, 2, FALSE)</f>
-        <v>11</v>
+        <f>VLOOKUP(A14, '2019'!A:B, 2, FALSE)</f>
+        <v>12</v>
       </c>
       <c r="D14">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E14" t="str">
         <f t="shared" si="1"/>
-        <v>d 2</v>
+        <v>d 1</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15">
-        <f>VLOOKUP(A15, '2018'!A:B, 2, FALSE)</f>
+        <f>VLOOKUP(A15, '2019'!A:B, 2, FALSE)</f>
         <v>13</v>
       </c>
       <c r="D15">
@@ -12908,202 +14962,202 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16">
-        <f>VLOOKUP(A16, '2018'!A:B, 2, FALSE)</f>
-        <v>15</v>
+        <f>VLOOKUP(A16, '2019'!A:B, 2, FALSE)</f>
+        <v>16</v>
       </c>
       <c r="D16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E16" t="str">
         <f t="shared" si="1"/>
-        <v>-</v>
+        <v>u 1</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17">
-        <f>VLOOKUP(A17, '2018'!A:B, 2, FALSE)</f>
-        <v>21</v>
+        <f>VLOOKUP(A17, '2019'!A:B, 2, FALSE)</f>
+        <v>10</v>
       </c>
       <c r="D17">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>-6</v>
       </c>
       <c r="E17" t="str">
         <f t="shared" si="1"/>
-        <v>u 5</v>
+        <v>d 6</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18">
-        <f>VLOOKUP(A18, '2018'!A:B, 2, FALSE)</f>
-        <v>16</v>
+        <f>VLOOKUP(A18, '2019'!A:B, 2, FALSE)</f>
+        <v>32</v>
       </c>
       <c r="D18">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>15</v>
       </c>
       <c r="E18" t="str">
         <f t="shared" si="1"/>
-        <v>d 1</v>
+        <v>u 15</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19">
-        <f>VLOOKUP(A19, '2018'!A:B, 2, FALSE)</f>
-        <v>10</v>
+        <f>VLOOKUP(A19, '2019'!A:B, 2, FALSE)</f>
+        <v>21</v>
       </c>
       <c r="D19">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>3</v>
       </c>
       <c r="E19" t="str">
         <f t="shared" si="1"/>
-        <v>d 8</v>
+        <v>u 3</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20">
-        <f>VLOOKUP(A20, '2018'!A:B, 2, FALSE)</f>
-        <v>19</v>
+        <f>VLOOKUP(A20, '2019'!A:B, 2, FALSE)</f>
+        <v>23</v>
       </c>
       <c r="D20">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E20" t="str">
         <f t="shared" si="1"/>
-        <v>-</v>
+        <v>u 4</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21">
-        <f>VLOOKUP(A21, '2018'!A:B, 2, FALSE)</f>
-        <v>18</v>
+        <f>VLOOKUP(A21, '2019'!A:B, 2, FALSE)</f>
+        <v>17</v>
       </c>
       <c r="D21">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="E21" t="str">
         <f t="shared" si="1"/>
-        <v>d 2</v>
+        <v>d 3</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22">
-        <f>VLOOKUP(A22, '2018'!A:B, 2, FALSE)</f>
-        <v>20</v>
+        <f>VLOOKUP(A22, '2019'!A:B, 2, FALSE)</f>
+        <v>22</v>
       </c>
       <c r="D22">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="E22" t="str">
         <f t="shared" si="1"/>
-        <v>d 1</v>
+        <v>u 1</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23">
-        <f>VLOOKUP(A23, '2018'!A:B, 2, FALSE)</f>
-        <v>28</v>
+        <f>VLOOKUP(A23, '2019'!A:B, 2, FALSE)</f>
+        <v>19</v>
       </c>
       <c r="D23">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>-3</v>
       </c>
       <c r="E23" t="str">
         <f t="shared" si="1"/>
-        <v>u 6</v>
+        <v>d 3</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24">
-        <f>VLOOKUP(A24, '2018'!A:B, 2, FALSE)</f>
-        <v>26</v>
+        <f>VLOOKUP(A24, '2019'!A:B, 2, FALSE)</f>
+        <v>18</v>
       </c>
       <c r="D24">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>-5</v>
       </c>
       <c r="E24" t="str">
         <f t="shared" si="1"/>
-        <v>u 3</v>
+        <v>d 5</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25">
-        <f>VLOOKUP(A25, '2018'!A:B, 2, FALSE)</f>
-        <v>25</v>
+        <f>VLOOKUP(A25, '2019'!A:B, 2, FALSE)</f>
+        <v>20</v>
       </c>
       <c r="D25">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="E25" t="str">
         <f t="shared" si="1"/>
-        <v>u 1</v>
+        <v>d 4</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -13114,96 +15168,96 @@
         <v>25</v>
       </c>
       <c r="C26">
-        <f>VLOOKUP(A26, '2018'!A:B, 2, FALSE)</f>
-        <v>22</v>
+        <f>VLOOKUP(A26, '2019'!A:B, 2, FALSE)</f>
+        <v>25</v>
       </c>
       <c r="D26">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>0</v>
       </c>
       <c r="E26" t="str">
         <f t="shared" si="1"/>
-        <v>d 3</v>
+        <v>-</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
       <c r="C27">
-        <f>VLOOKUP(A27, '2018'!A:B, 2, FALSE)</f>
-        <v>23</v>
+        <f>VLOOKUP(A27, '2019'!A:B, 2, FALSE)</f>
+        <v>24</v>
       </c>
       <c r="D27">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-2</v>
       </c>
       <c r="E27" t="str">
         <f t="shared" si="1"/>
-        <v>d 3</v>
+        <v>d 2</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
       <c r="C28">
-        <f>VLOOKUP(A28, '2018'!A:B, 2, FALSE)</f>
-        <v>24</v>
+        <f>VLOOKUP(A28, '2019'!A:B, 2, FALSE)</f>
+        <v>28</v>
       </c>
       <c r="D28">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>1</v>
       </c>
       <c r="E28" t="str">
         <f t="shared" si="1"/>
-        <v>d 3</v>
+        <v>u 1</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
       <c r="C29">
-        <f>VLOOKUP(A29, '2018'!A:B, 2, FALSE)</f>
-        <v>27</v>
+        <f>VLOOKUP(A29, '2019'!A:B, 2, FALSE)</f>
+        <v>31</v>
       </c>
       <c r="D29">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="E29" t="str">
         <f t="shared" si="1"/>
-        <v>d 1</v>
+        <v>u 3</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
       <c r="C30">
-        <f>VLOOKUP(A30, '2018'!A:B, 2, FALSE)</f>
-        <v>29</v>
+        <f>VLOOKUP(A30, '2019'!A:B, 2, FALSE)</f>
+        <v>26</v>
       </c>
       <c r="D30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-3</v>
       </c>
       <c r="E30" t="str">
         <f t="shared" si="1"/>
-        <v>-</v>
+        <v>d 3</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -13214,116 +15268,116 @@
         <v>30</v>
       </c>
       <c r="C31">
-        <f>VLOOKUP(A31, '2018'!A:B, 2, FALSE)</f>
-        <v>33</v>
+        <f>VLOOKUP(A31, '2019'!A:B, 2, FALSE)</f>
+        <v>30</v>
       </c>
       <c r="D31">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E31" t="str">
         <f t="shared" si="1"/>
-        <v>u 3</v>
+        <v>-</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B32">
         <v>31</v>
       </c>
       <c r="C32">
-        <f>VLOOKUP(A32, '2018'!A:B, 2, FALSE)</f>
-        <v>34</v>
+        <f>VLOOKUP(A32, '2019'!A:B, 2, FALSE)</f>
+        <v>39</v>
       </c>
       <c r="D32">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E32" t="str">
         <f t="shared" si="1"/>
-        <v>u 3</v>
+        <v>u 8</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
       <c r="C33">
-        <f>VLOOKUP(A33, '2018'!A:B, 2, FALSE)</f>
-        <v>86</v>
+        <f>VLOOKUP(A33, '2019'!A:B, 2, FALSE)</f>
+        <v>35</v>
       </c>
       <c r="D33">
         <f t="shared" si="0"/>
-        <v>54</v>
+        <v>3</v>
       </c>
       <c r="E33" t="str">
         <f t="shared" si="1"/>
-        <v>u 54</v>
+        <v>u 3</v>
       </c>
     </row>
     <row r="34" spans="1:5">
       <c r="A34" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B34">
         <v>33</v>
       </c>
       <c r="C34">
-        <f>VLOOKUP(A34, '2018'!A:B, 2, FALSE)</f>
-        <v>45</v>
+        <f>VLOOKUP(A34, '2019'!A:B, 2, FALSE)</f>
+        <v>38</v>
       </c>
       <c r="D34">
         <f t="shared" si="0"/>
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="E34" t="str">
         <f t="shared" si="1"/>
-        <v>u 12</v>
+        <v>u 5</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="B35">
         <v>34</v>
       </c>
       <c r="C35">
-        <f>VLOOKUP(A35, '2018'!A:B, 2, FALSE)</f>
-        <v>32</v>
+        <f>VLOOKUP(A35, '2019'!A:B, 2, FALSE)</f>
+        <v>33</v>
       </c>
       <c r="D35">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="E35" t="str">
         <f t="shared" si="1"/>
-        <v>d 2</v>
+        <v>d 1</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="B36">
         <v>35</v>
       </c>
       <c r="C36">
-        <f>VLOOKUP(A36, '2018'!A:B, 2, FALSE)</f>
-        <v>30</v>
+        <f>VLOOKUP(A36, '2019'!A:B, 2, FALSE)</f>
+        <v>27</v>
       </c>
       <c r="D36">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>-8</v>
       </c>
       <c r="E36" t="str">
         <f t="shared" si="1"/>
-        <v>d 5</v>
+        <v>d 8</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -13334,407 +15388,407 @@
         <v>36</v>
       </c>
       <c r="C37">
-        <f>VLOOKUP(A37, '2018'!A:B, 2, FALSE)</f>
-        <v>38</v>
+        <f>VLOOKUP(A37, '2019'!A:B, 2, FALSE)</f>
+        <v>36</v>
       </c>
       <c r="D37">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E37" t="str">
         <f t="shared" si="1"/>
-        <v>u 2</v>
+        <v>-</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B38">
         <v>37</v>
       </c>
       <c r="C38">
-        <f>VLOOKUP(A38, '2018'!A:B, 2, FALSE)</f>
-        <v>31</v>
+        <f>VLOOKUP(A38, '2019'!A:B, 2, FALSE)</f>
+        <v>40</v>
       </c>
       <c r="D38">
         <f t="shared" si="0"/>
-        <v>-6</v>
+        <v>3</v>
       </c>
       <c r="E38" t="str">
         <f t="shared" si="1"/>
-        <v>d 6</v>
+        <v>u 3</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B39">
         <v>38</v>
       </c>
       <c r="C39">
-        <f>VLOOKUP(A39, '2018'!A:B, 2, FALSE)</f>
-        <v>36</v>
+        <f>VLOOKUP(A39, '2019'!A:B, 2, FALSE)</f>
+        <v>42</v>
       </c>
       <c r="D39">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>4</v>
       </c>
       <c r="E39" t="str">
         <f t="shared" si="1"/>
-        <v>d 2</v>
+        <v>u 4</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="B40">
         <v>39</v>
       </c>
       <c r="C40">
-        <f>VLOOKUP(A40, '2018'!A:B, 2, FALSE)</f>
-        <v>49</v>
+        <f>VLOOKUP(A40, '2019'!A:B, 2, FALSE)</f>
+        <v>37</v>
       </c>
       <c r="D40">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>-2</v>
       </c>
       <c r="E40" t="str">
         <f t="shared" si="1"/>
-        <v>u 10</v>
+        <v>d 2</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B41">
         <v>40</v>
       </c>
       <c r="C41">
-        <f>VLOOKUP(A41, '2018'!A:B, 2, FALSE)</f>
-        <v>42</v>
+        <f>VLOOKUP(A41, '2019'!A:B, 2, FALSE)</f>
+        <v>29</v>
       </c>
       <c r="D41">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>-11</v>
       </c>
       <c r="E41" t="str">
         <f t="shared" si="1"/>
-        <v>u 2</v>
+        <v>d 11</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="B42">
         <v>41</v>
       </c>
       <c r="C42">
-        <f>VLOOKUP(A42, '2018'!A:B, 2, FALSE)</f>
-        <v>48</v>
+        <f>VLOOKUP(A42, '2019'!A:B, 2, FALSE)</f>
+        <v>60</v>
       </c>
       <c r="D42">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>19</v>
       </c>
       <c r="E42" t="str">
         <f t="shared" si="1"/>
-        <v>u 7</v>
+        <v>u 19</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B43">
         <v>42</v>
       </c>
       <c r="C43">
-        <f>VLOOKUP(A43, '2018'!A:B, 2, FALSE)</f>
-        <v>41</v>
+        <f>VLOOKUP(A43, '2019'!A:B, 2, FALSE)</f>
+        <v>44</v>
       </c>
       <c r="D43">
         <f t="shared" si="0"/>
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="E43" t="str">
         <f t="shared" si="1"/>
-        <v>d 1</v>
+        <v>u 2</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B44">
         <v>43</v>
       </c>
       <c r="C44">
-        <f>VLOOKUP(A44, '2018'!A:B, 2, FALSE)</f>
-        <v>35</v>
+        <f>VLOOKUP(A44, '2019'!A:B, 2, FALSE)</f>
+        <v>41</v>
       </c>
       <c r="D44">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>-2</v>
       </c>
       <c r="E44" t="str">
         <f t="shared" si="1"/>
-        <v>d 8</v>
+        <v>d 2</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B45">
         <v>44</v>
       </c>
       <c r="C45">
-        <f>VLOOKUP(A45, '2018'!A:B, 2, FALSE)</f>
-        <v>67</v>
+        <f>VLOOKUP(A45, '2019'!A:B, 2, FALSE)</f>
+        <v>34</v>
       </c>
       <c r="D45">
         <f t="shared" si="0"/>
-        <v>23</v>
+        <v>-10</v>
       </c>
       <c r="E45" t="str">
         <f t="shared" si="1"/>
-        <v>u 23</v>
+        <v>d 10</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B46">
         <v>45</v>
       </c>
       <c r="C46">
-        <f>VLOOKUP(A46, '2018'!A:B, 2, FALSE)</f>
-        <v>40</v>
+        <f>VLOOKUP(A46, '2019'!A:B, 2, FALSE)</f>
+        <v>52</v>
       </c>
       <c r="D46">
         <f t="shared" si="0"/>
-        <v>-5</v>
+        <v>7</v>
       </c>
       <c r="E46" t="str">
         <f t="shared" si="1"/>
-        <v>d 5</v>
+        <v>u 7</v>
       </c>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B47">
         <v>46</v>
       </c>
       <c r="C47">
-        <f>VLOOKUP(A47, '2018'!A:B, 2, FALSE)</f>
-        <v>46</v>
+        <f>VLOOKUP(A47, '2019'!A:B, 2, FALSE)</f>
+        <v>56</v>
       </c>
       <c r="D47">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E47" t="str">
         <f t="shared" si="1"/>
-        <v>-</v>
+        <v>u 10</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="B48">
         <v>47</v>
       </c>
       <c r="C48">
-        <f>VLOOKUP(A48, '2018'!A:B, 2, FALSE)</f>
-        <v>71</v>
+        <f>VLOOKUP(A48, '2019'!A:B, 2, FALSE)</f>
+        <v>49</v>
       </c>
       <c r="D48">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>2</v>
       </c>
       <c r="E48" t="str">
         <f t="shared" si="1"/>
-        <v>u 24</v>
+        <v>u 2</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" t="s">
-        <v>59</v>
+        <v>45</v>
       </c>
       <c r="B49">
         <v>48</v>
       </c>
       <c r="C49">
-        <f>VLOOKUP(A49, '2018'!A:B, 2, FALSE)</f>
-        <v>37</v>
+        <f>VLOOKUP(A49, '2019'!A:B, 2, FALSE)</f>
+        <v>47</v>
       </c>
       <c r="D49">
         <f t="shared" si="0"/>
-        <v>-11</v>
+        <v>-1</v>
       </c>
       <c r="E49" t="str">
         <f t="shared" si="1"/>
-        <v>d 11</v>
+        <v>d 1</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B50">
         <v>49</v>
       </c>
       <c r="C50">
-        <f>VLOOKUP(A50, '2018'!A:B, 2, FALSE)</f>
-        <v>58</v>
+        <f>VLOOKUP(A50, '2019'!A:B, 2, FALSE)</f>
+        <v>43</v>
       </c>
       <c r="D50">
         <f t="shared" si="0"/>
-        <v>9</v>
+        <v>-6</v>
       </c>
       <c r="E50" t="str">
         <f t="shared" si="1"/>
-        <v>u 9</v>
+        <v>d 6</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B51">
         <v>50</v>
       </c>
       <c r="C51">
-        <f>VLOOKUP(A51, '2018'!A:B, 2, FALSE)</f>
-        <v>51</v>
+        <f>VLOOKUP(A51, '2019'!A:B, 2, FALSE)</f>
+        <v>46</v>
       </c>
       <c r="D51">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>-4</v>
       </c>
       <c r="E51" t="str">
         <f t="shared" si="1"/>
-        <v>u 1</v>
+        <v>d 4</v>
       </c>
     </row>
     <row r="52" spans="1:5">
       <c r="A52" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B52">
         <v>51</v>
       </c>
       <c r="C52">
-        <f>VLOOKUP(A52, '2018'!A:B, 2, FALSE)</f>
-        <v>52</v>
+        <f>VLOOKUP(A52, '2019'!A:B, 2, FALSE)</f>
+        <v>55</v>
       </c>
       <c r="D52">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E52" t="str">
         <f t="shared" si="1"/>
-        <v>u 1</v>
+        <v>u 4</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B53">
         <v>52</v>
       </c>
       <c r="C53">
-        <f>VLOOKUP(A53, '2018'!A:B, 2, FALSE)</f>
-        <v>44</v>
+        <f>VLOOKUP(A53, '2019'!A:B, 2, FALSE)</f>
+        <v>45</v>
       </c>
       <c r="D53">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>-7</v>
       </c>
       <c r="E53" t="str">
         <f t="shared" si="1"/>
-        <v>d 8</v>
+        <v>d 7</v>
       </c>
     </row>
     <row r="54" spans="1:5">
       <c r="A54" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B54">
         <v>53</v>
       </c>
       <c r="C54">
-        <f>VLOOKUP(A54, '2018'!A:B, 2, FALSE)</f>
-        <v>39</v>
+        <f>VLOOKUP(A54, '2019'!A:B, 2, FALSE)</f>
+        <v>70</v>
       </c>
       <c r="D54">
         <f t="shared" si="0"/>
-        <v>-14</v>
+        <v>17</v>
       </c>
       <c r="E54" t="str">
         <f t="shared" si="1"/>
-        <v>d 14</v>
+        <v>u 17</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="B55">
         <v>54</v>
       </c>
       <c r="C55">
-        <f>VLOOKUP(A55, '2018'!A:B, 2, FALSE)</f>
-        <v>62</v>
+        <f>VLOOKUP(A55, '2019'!A:B, 2, FALSE)</f>
+        <v>63</v>
       </c>
       <c r="D55">
         <f t="shared" si="0"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E55" t="str">
         <f t="shared" si="1"/>
-        <v>u 8</v>
+        <v>u 9</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B56">
         <v>55</v>
       </c>
       <c r="C56">
-        <f>VLOOKUP(A56, '2018'!A:B, 2, FALSE)</f>
-        <v>53</v>
+        <f>VLOOKUP(A56, '2019'!A:B, 2, FALSE)</f>
+        <v>57</v>
       </c>
       <c r="D56">
         <f t="shared" si="0"/>
-        <v>-2</v>
+        <v>2</v>
       </c>
       <c r="E56" t="str">
         <f t="shared" si="1"/>
-        <v>d 2</v>
+        <v>u 2</v>
       </c>
     </row>
     <row r="57" spans="1:5">
       <c r="A57" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
       <c r="B57">
         <v>56</v>
       </c>
       <c r="C57">
-        <f>VLOOKUP(A57, '2018'!A:B, 2, FALSE)</f>
+        <f>VLOOKUP(A57, '2019'!A:B, 2, FALSE)</f>
         <v>61</v>
       </c>
       <c r="D57">
@@ -13748,142 +15802,142 @@
     </row>
     <row r="58" spans="1:5">
       <c r="A58" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="B58">
         <v>57</v>
       </c>
       <c r="C58">
-        <f>VLOOKUP(A58, '2018'!A:B, 2, FALSE)</f>
-        <v>47</v>
+        <f>VLOOKUP(A58, '2019'!A:B, 2, FALSE)</f>
+        <v>81</v>
       </c>
       <c r="D58">
         <f t="shared" si="0"/>
-        <v>-10</v>
+        <v>24</v>
       </c>
       <c r="E58" t="str">
         <f t="shared" si="1"/>
-        <v>d 10</v>
+        <v>u 24</v>
       </c>
     </row>
     <row r="59" spans="1:5">
       <c r="A59" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B59">
         <v>58</v>
       </c>
       <c r="C59">
-        <f>VLOOKUP(A59, '2018'!A:B, 2, FALSE)</f>
-        <v>55</v>
+        <f>VLOOKUP(A59, '2019'!A:B, 2, FALSE)</f>
+        <v>51</v>
       </c>
       <c r="D59">
         <f t="shared" si="0"/>
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="E59" t="str">
         <f t="shared" si="1"/>
-        <v>d 3</v>
+        <v>d 7</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="B60">
         <v>59</v>
       </c>
       <c r="C60">
-        <f>VLOOKUP(A60, '2018'!A:B, 2, FALSE)</f>
-        <v>43</v>
+        <f>VLOOKUP(A60, '2019'!A:B, 2, FALSE)</f>
+        <v>54</v>
       </c>
       <c r="D60">
         <f t="shared" si="0"/>
-        <v>-16</v>
+        <v>-5</v>
       </c>
       <c r="E60" t="str">
         <f t="shared" si="1"/>
-        <v>d 16</v>
+        <v>d 5</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="B61">
         <v>60</v>
       </c>
-      <c r="C61" t="e">
-        <f>VLOOKUP(A61, '2018'!A:B, 2, FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D61" t="e">
-        <f t="shared" si="0"/>
-        <v>#N/A</v>
+      <c r="C61">
+        <f>VLOOKUP(A61, '2019'!A:B, 2, FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>-10</v>
       </c>
       <c r="E61" t="str">
         <f t="shared" si="1"/>
-        <v>new</v>
+        <v>d 10</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="B62">
         <v>61</v>
       </c>
       <c r="C62">
-        <f>VLOOKUP(A62, '2018'!A:B, 2, FALSE)</f>
-        <v>63</v>
+        <f>VLOOKUP(A62, '2019'!A:B, 2, FALSE)</f>
+        <v>58</v>
       </c>
       <c r="D62">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>-3</v>
       </c>
       <c r="E62" t="str">
         <f t="shared" si="1"/>
-        <v>u 2</v>
+        <v>d 3</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B63">
         <v>62</v>
       </c>
       <c r="C63">
-        <f>VLOOKUP(A63, '2018'!A:B, 2, FALSE)</f>
-        <v>54</v>
+        <f>VLOOKUP(A63, '2019'!A:B, 2, FALSE)</f>
+        <v>66</v>
       </c>
       <c r="D63">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>4</v>
       </c>
       <c r="E63" t="str">
         <f t="shared" si="1"/>
-        <v>d 8</v>
+        <v>u 4</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="B64">
         <v>63</v>
       </c>
       <c r="C64">
-        <f>VLOOKUP(A64, '2018'!A:B, 2, FALSE)</f>
-        <v>68</v>
+        <f>VLOOKUP(A64, '2019'!A:B, 2, FALSE)</f>
+        <v>73</v>
       </c>
       <c r="D64">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E64" t="str">
         <f t="shared" si="1"/>
-        <v>u 5</v>
+        <v>u 10</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -13894,187 +15948,187 @@
         <v>64</v>
       </c>
       <c r="C65">
-        <f>VLOOKUP(A65, '2018'!A:B, 2, FALSE)</f>
-        <v>65</v>
+        <f>VLOOKUP(A65, '2019'!A:B, 2, FALSE)</f>
+        <v>64</v>
       </c>
       <c r="D65">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E65" t="str">
         <f t="shared" si="1"/>
-        <v>u 1</v>
+        <v>-</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B66">
         <v>65</v>
       </c>
       <c r="C66">
-        <f>VLOOKUP(A66, '2018'!A:B, 2, FALSE)</f>
-        <v>57</v>
+        <f>VLOOKUP(A66, '2019'!A:B, 2, FALSE)</f>
+        <v>78</v>
       </c>
       <c r="D66">
         <f t="shared" si="0"/>
-        <v>-8</v>
+        <v>13</v>
       </c>
       <c r="E66" t="str">
         <f t="shared" si="1"/>
-        <v>d 8</v>
+        <v>u 13</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B67">
         <v>66</v>
       </c>
       <c r="C67">
-        <f>VLOOKUP(A67, '2018'!A:B, 2, FALSE)</f>
-        <v>92</v>
+        <f>VLOOKUP(A67, '2019'!A:B, 2, FALSE)</f>
+        <v>48</v>
       </c>
       <c r="D67">
         <f t="shared" ref="D67:D101" si="2">C67-B67</f>
-        <v>26</v>
+        <v>-18</v>
       </c>
       <c r="E67" t="str">
         <f t="shared" ref="E67:E101" si="3">IF(ISNA(D67), "new", IF(D67 = 0, "-", IF(D67 &gt; 0, CONCATENATE("u ", D67),   IF(D67 &lt; 0, CONCATENATE("d ", ABS(D67))))))</f>
-        <v>u 26</v>
+        <v>d 18</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B68">
         <v>67</v>
       </c>
       <c r="C68">
-        <f>VLOOKUP(A68, '2018'!A:B, 2, FALSE)</f>
-        <v>56</v>
+        <f>VLOOKUP(A68, '2019'!A:B, 2, FALSE)</f>
+        <v>53</v>
       </c>
       <c r="D68">
         <f t="shared" si="2"/>
-        <v>-11</v>
+        <v>-14</v>
       </c>
       <c r="E68" t="str">
         <f t="shared" si="3"/>
-        <v>d 11</v>
+        <v>d 14</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="B69">
         <v>68</v>
       </c>
       <c r="C69">
-        <f>VLOOKUP(A69, '2018'!A:B, 2, FALSE)</f>
-        <v>60</v>
+        <f>VLOOKUP(A69, '2019'!A:B, 2, FALSE)</f>
+        <v>62</v>
       </c>
       <c r="D69">
         <f t="shared" si="2"/>
-        <v>-8</v>
+        <v>-6</v>
       </c>
       <c r="E69" t="str">
         <f t="shared" si="3"/>
-        <v>d 8</v>
+        <v>d 6</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" t="s">
-        <v>95</v>
+        <v>69</v>
       </c>
       <c r="B70">
         <v>69</v>
       </c>
       <c r="C70">
-        <f>VLOOKUP(A70, '2018'!A:B, 2, FALSE)</f>
-        <v>76</v>
+        <f>VLOOKUP(A70, '2019'!A:B, 2, FALSE)</f>
+        <v>74</v>
       </c>
       <c r="D70">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E70" t="str">
         <f t="shared" si="3"/>
-        <v>u 7</v>
+        <v>u 5</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" t="s">
-        <v>63</v>
+        <v>90</v>
       </c>
       <c r="B71">
         <v>70</v>
       </c>
       <c r="C71">
-        <f>VLOOKUP(A71, '2018'!A:B, 2, FALSE)</f>
-        <v>73</v>
+        <f>VLOOKUP(A71, '2019'!A:B, 2, FALSE)</f>
+        <v>94</v>
       </c>
       <c r="D71">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E71" t="str">
         <f t="shared" si="3"/>
-        <v>u 3</v>
+        <v>u 24</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="B72">
         <v>71</v>
       </c>
       <c r="C72">
-        <f>VLOOKUP(A72, '2018'!A:B, 2, FALSE)</f>
-        <v>59</v>
+        <f>VLOOKUP(A72, '2019'!A:B, 2, FALSE)</f>
+        <v>76</v>
       </c>
       <c r="D72">
         <f t="shared" si="2"/>
-        <v>-12</v>
+        <v>5</v>
       </c>
       <c r="E72" t="str">
         <f t="shared" si="3"/>
-        <v>d 12</v>
+        <v>u 5</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" t="s">
-        <v>74</v>
+        <v>86</v>
       </c>
       <c r="B73">
         <v>72</v>
       </c>
       <c r="C73">
-        <f>VLOOKUP(A73, '2018'!A:B, 2, FALSE)</f>
-        <v>96</v>
+        <f>VLOOKUP(A73, '2019'!A:B, 2, FALSE)</f>
+        <v>90</v>
       </c>
       <c r="D73">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E73" t="str">
         <f t="shared" si="3"/>
-        <v>u 24</v>
+        <v>u 18</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B74">
         <v>73</v>
       </c>
       <c r="C74">
-        <f>VLOOKUP(A74, '2018'!A:B, 2, FALSE)</f>
+        <f>VLOOKUP(A74, '2019'!A:B, 2, FALSE)</f>
         <v>75</v>
       </c>
       <c r="D74">
@@ -14088,13 +16142,13 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="B75">
         <v>74</v>
       </c>
       <c r="C75">
-        <f>VLOOKUP(A75, '2018'!A:B, 2, FALSE)</f>
+        <f>VLOOKUP(A75, '2019'!A:B, 2, FALSE)</f>
         <v>72</v>
       </c>
       <c r="D75">
@@ -14108,13 +16162,13 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" t="s">
-        <v>68</v>
+        <v>89</v>
       </c>
       <c r="B76">
         <v>75</v>
       </c>
       <c r="C76" t="e">
-        <f>VLOOKUP(A76, '2018'!A:B, 2, FALSE)</f>
+        <f>VLOOKUP(A76, '2019'!A:B, 2, FALSE)</f>
         <v>#N/A</v>
       </c>
       <c r="D76" t="e">
@@ -14128,122 +16182,122 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B77">
         <v>76</v>
       </c>
       <c r="C77">
-        <f>VLOOKUP(A77, '2018'!A:B, 2, FALSE)</f>
-        <v>78</v>
+        <f>VLOOKUP(A77, '2019'!A:B, 2, FALSE)</f>
+        <v>65</v>
       </c>
       <c r="D77">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>-11</v>
       </c>
       <c r="E77" t="str">
         <f t="shared" si="3"/>
-        <v>u 2</v>
+        <v>d 11</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" t="s">
-        <v>79</v>
+        <v>91</v>
       </c>
       <c r="B78">
         <v>77</v>
       </c>
       <c r="C78">
-        <f>VLOOKUP(A78, '2018'!A:B, 2, FALSE)</f>
-        <v>69</v>
+        <f>VLOOKUP(A78, '2019'!A:B, 2, FALSE)</f>
+        <v>95</v>
       </c>
       <c r="D78">
         <f t="shared" si="2"/>
-        <v>-8</v>
+        <v>18</v>
       </c>
       <c r="E78" t="str">
         <f t="shared" si="3"/>
-        <v>d 8</v>
+        <v>u 18</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B79">
         <v>78</v>
       </c>
       <c r="C79">
-        <f>VLOOKUP(A79, '2018'!A:B, 2, FALSE)</f>
-        <v>87</v>
+        <f>VLOOKUP(A79, '2019'!A:B, 2, FALSE)</f>
+        <v>59</v>
       </c>
       <c r="D79">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>-19</v>
       </c>
       <c r="E79" t="str">
         <f t="shared" si="3"/>
-        <v>u 9</v>
+        <v>d 19</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" t="s">
-        <v>98</v>
+        <v>84</v>
       </c>
       <c r="B80">
         <v>79</v>
       </c>
       <c r="C80">
-        <f>VLOOKUP(A80, '2018'!A:B, 2, FALSE)</f>
-        <v>70</v>
+        <f>VLOOKUP(A80, '2019'!A:B, 2, FALSE)</f>
+        <v>83</v>
       </c>
       <c r="D80">
         <f t="shared" si="2"/>
-        <v>-9</v>
+        <v>4</v>
       </c>
       <c r="E80" t="str">
         <f t="shared" si="3"/>
-        <v>d 9</v>
+        <v>u 4</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B81">
         <v>80</v>
       </c>
       <c r="C81">
-        <f>VLOOKUP(A81, '2018'!A:B, 2, FALSE)</f>
-        <v>79</v>
+        <f>VLOOKUP(A81, '2019'!A:B, 2, FALSE)</f>
+        <v>89</v>
       </c>
       <c r="D81">
         <f t="shared" si="2"/>
-        <v>-1</v>
+        <v>9</v>
       </c>
       <c r="E81" t="str">
         <f t="shared" si="3"/>
-        <v>d 1</v>
+        <v>u 9</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" t="s">
-        <v>66</v>
+        <v>79</v>
       </c>
       <c r="B82">
         <v>81</v>
       </c>
       <c r="C82">
-        <f>VLOOKUP(A82, '2018'!A:B, 2, FALSE)</f>
-        <v>64</v>
+        <f>VLOOKUP(A82, '2019'!A:B, 2, FALSE)</f>
+        <v>77</v>
       </c>
       <c r="D82">
         <f t="shared" si="2"/>
-        <v>-17</v>
+        <v>-4</v>
       </c>
       <c r="E82" t="str">
         <f t="shared" si="3"/>
-        <v>d 17</v>
+        <v>d 4</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -14254,7 +16308,7 @@
         <v>82</v>
       </c>
       <c r="C83">
-        <f>VLOOKUP(A83, '2018'!A:B, 2, FALSE)</f>
+        <f>VLOOKUP(A83, '2019'!A:B, 2, FALSE)</f>
         <v>82</v>
       </c>
       <c r="D83">
@@ -14268,362 +16322,362 @@
     </row>
     <row r="84" spans="1:5">
       <c r="A84" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B84">
         <v>83</v>
       </c>
       <c r="C84">
-        <f>VLOOKUP(A84, '2018'!A:B, 2, FALSE)</f>
-        <v>81</v>
+        <f>VLOOKUP(A84, '2019'!A:B, 2, FALSE)</f>
+        <v>88</v>
       </c>
       <c r="D84">
         <f t="shared" si="2"/>
-        <v>-2</v>
+        <v>5</v>
       </c>
       <c r="E84" t="str">
         <f t="shared" si="3"/>
-        <v>d 2</v>
+        <v>u 5</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" t="s">
-        <v>75</v>
+        <v>92</v>
       </c>
       <c r="B85">
         <v>84</v>
       </c>
       <c r="C85">
-        <f>VLOOKUP(A85, '2018'!A:B, 2, FALSE)</f>
-        <v>88</v>
+        <f>VLOOKUP(A85, '2019'!A:B, 2, FALSE)</f>
+        <v>87</v>
       </c>
       <c r="D85">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E85" t="str">
         <f t="shared" si="3"/>
-        <v>u 4</v>
+        <v>u 3</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B86">
         <v>85</v>
       </c>
       <c r="C86">
-        <f>VLOOKUP(A86, '2018'!A:B, 2, FALSE)</f>
-        <v>74</v>
+        <f>VLOOKUP(A86, '2019'!A:B, 2, FALSE)</f>
+        <v>69</v>
       </c>
       <c r="D86">
         <f t="shared" si="2"/>
-        <v>-11</v>
+        <v>-16</v>
       </c>
       <c r="E86" t="str">
         <f t="shared" si="3"/>
-        <v>d 11</v>
+        <v>d 16</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B87">
         <v>86</v>
       </c>
-      <c r="C87">
-        <f>VLOOKUP(A87, '2018'!A:B, 2, FALSE)</f>
-        <v>77</v>
-      </c>
-      <c r="D87">
-        <f t="shared" si="2"/>
-        <v>-9</v>
+      <c r="C87" t="e">
+        <f>VLOOKUP(A87, '2019'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D87" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
       </c>
       <c r="E87" t="str">
         <f t="shared" si="3"/>
-        <v>d 9</v>
+        <v>new</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" t="s">
-        <v>92</v>
+        <v>75</v>
       </c>
       <c r="B88">
         <v>87</v>
       </c>
       <c r="C88">
-        <f>VLOOKUP(A88, '2018'!A:B, 2, FALSE)</f>
-        <v>83</v>
+        <f>VLOOKUP(A88, '2019'!A:B, 2, FALSE)</f>
+        <v>84</v>
       </c>
       <c r="D88">
         <f t="shared" si="2"/>
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="E88" t="str">
         <f t="shared" si="3"/>
-        <v>d 4</v>
+        <v>d 3</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="B89">
         <v>88</v>
       </c>
-      <c r="C89" t="e">
-        <f>VLOOKUP(A89, '2018'!A:B, 2, FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D89" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="C89">
+        <f>VLOOKUP(A89, '2019'!A:B, 2, FALSE)</f>
+        <v>91</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="2"/>
+        <v>3</v>
       </c>
       <c r="E89" t="str">
         <f t="shared" si="3"/>
-        <v>new</v>
+        <v>u 3</v>
       </c>
     </row>
     <row r="90" spans="1:5">
       <c r="A90" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="B90">
         <v>89</v>
       </c>
-      <c r="C90">
-        <f>VLOOKUP(A90, '2018'!A:B, 2, FALSE)</f>
-        <v>95</v>
-      </c>
-      <c r="D90">
-        <f t="shared" si="2"/>
-        <v>6</v>
+      <c r="C90" t="e">
+        <f>VLOOKUP(A90, '2019'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D90" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
       </c>
       <c r="E90" t="str">
         <f t="shared" si="3"/>
-        <v>u 6</v>
+        <v>new</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B91">
         <v>90</v>
       </c>
-      <c r="C91" t="e">
-        <f>VLOOKUP(A91, '2018'!A:B, 2, FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D91" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="C91">
+        <f>VLOOKUP(A91, '2019'!A:B, 2, FALSE)</f>
+        <v>80</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="2"/>
+        <v>-10</v>
       </c>
       <c r="E91" t="str">
         <f t="shared" si="3"/>
-        <v>new</v>
+        <v>d 10</v>
       </c>
     </row>
     <row r="92" spans="1:5">
       <c r="A92" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B92">
         <v>91</v>
       </c>
-      <c r="C92" t="e">
-        <f>VLOOKUP(A92, '2018'!A:B, 2, FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D92" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="C92">
+        <f>VLOOKUP(A92, '2019'!A:B, 2, FALSE)</f>
+        <v>71</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="2"/>
+        <v>-20</v>
       </c>
       <c r="E92" t="str">
         <f t="shared" si="3"/>
-        <v>new</v>
+        <v>d 20</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="B93">
         <v>92</v>
       </c>
-      <c r="C93" t="e">
-        <f>VLOOKUP(A93, '2018'!A:B, 2, FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D93" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="C93">
+        <f>VLOOKUP(A93, '2019'!A:B, 2, FALSE)</f>
+        <v>67</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="2"/>
+        <v>-25</v>
       </c>
       <c r="E93" t="str">
         <f t="shared" si="3"/>
-        <v>new</v>
+        <v>d 25</v>
       </c>
     </row>
     <row r="94" spans="1:5">
       <c r="A94" t="s">
-        <v>128</v>
+        <v>103</v>
       </c>
       <c r="B94">
         <v>93</v>
       </c>
-      <c r="C94">
-        <f>VLOOKUP(A94, '2018'!A:B, 2, FALSE)</f>
-        <v>90</v>
-      </c>
-      <c r="D94">
-        <f t="shared" si="2"/>
-        <v>-3</v>
+      <c r="C94" t="e">
+        <f>VLOOKUP(A94, '2019'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D94" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
       </c>
       <c r="E94" t="str">
         <f t="shared" si="3"/>
-        <v>d 3</v>
+        <v>new</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" t="s">
-        <v>90</v>
+        <v>96</v>
       </c>
       <c r="B95">
         <v>94</v>
       </c>
-      <c r="C95" t="e">
-        <f>VLOOKUP(A95, '2018'!A:B, 2, FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D95" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="C95">
+        <f>VLOOKUP(A95, '2019'!A:B, 2, FALSE)</f>
+        <v>85</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="2"/>
+        <v>-9</v>
       </c>
       <c r="E95" t="str">
         <f t="shared" si="3"/>
-        <v>new</v>
+        <v>d 9</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B96">
         <v>95</v>
       </c>
-      <c r="C96" t="e">
-        <f>VLOOKUP(A96, '2018'!A:B, 2, FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D96" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="C96">
+        <f>VLOOKUP(A96, '2019'!A:B, 2, FALSE)</f>
+        <v>92</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="2"/>
+        <v>-3</v>
       </c>
       <c r="E96" t="str">
         <f t="shared" si="3"/>
-        <v>new</v>
+        <v>d 3</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="B97">
         <v>96</v>
       </c>
-      <c r="C97" t="e">
-        <f>VLOOKUP(A97, '2018'!A:B, 2, FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D97" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="C97">
+        <f>VLOOKUP(A97, '2019'!A:B, 2, FALSE)</f>
+        <v>68</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="2"/>
+        <v>-28</v>
       </c>
       <c r="E97" t="str">
         <f t="shared" si="3"/>
-        <v>new</v>
+        <v>d 28</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="B98">
         <v>97</v>
       </c>
-      <c r="C98">
-        <f>VLOOKUP(A98, '2018'!A:B, 2, FALSE)</f>
-        <v>85</v>
-      </c>
-      <c r="D98">
-        <f t="shared" si="2"/>
-        <v>-12</v>
+      <c r="C98" t="e">
+        <f>VLOOKUP(A98, '2019'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D98" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
       </c>
       <c r="E98" t="str">
         <f t="shared" si="3"/>
-        <v>d 12</v>
+        <v>new</v>
       </c>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
       <c r="B99">
         <v>98</v>
       </c>
-      <c r="C99" t="e">
-        <f>VLOOKUP(A99, '2018'!A:B, 2, FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D99" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="C99">
+        <f>VLOOKUP(A99, '2019'!A:B, 2, FALSE)</f>
+        <v>86</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="2"/>
+        <v>-12</v>
       </c>
       <c r="E99" t="str">
         <f t="shared" si="3"/>
-        <v>new</v>
+        <v>d 12</v>
       </c>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="B100">
         <v>99</v>
       </c>
-      <c r="C100" t="e">
-        <f>VLOOKUP(A100, '2018'!A:B, 2, FALSE)</f>
-        <v>#N/A</v>
-      </c>
-      <c r="D100" t="e">
-        <f t="shared" si="2"/>
-        <v>#N/A</v>
+      <c r="C100">
+        <f>VLOOKUP(A100, '2019'!A:B, 2, FALSE)</f>
+        <v>98</v>
+      </c>
+      <c r="D100">
+        <f t="shared" si="2"/>
+        <v>-1</v>
       </c>
       <c r="E100" t="str">
         <f t="shared" si="3"/>
-        <v>new</v>
+        <v>d 1</v>
       </c>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" t="s">
-        <v>126</v>
+        <v>99</v>
       </c>
       <c r="B101">
         <v>100</v>
       </c>
       <c r="C101">
-        <f>VLOOKUP(A101, '2018'!A:B, 2, FALSE)</f>
-        <v>84</v>
+        <f>VLOOKUP(A101, '2019'!A:B, 2, FALSE)</f>
+        <v>96</v>
       </c>
       <c r="D101">
         <f t="shared" si="2"/>
-        <v>-16</v>
+        <v>-4</v>
       </c>
       <c r="E101" t="str">
         <f t="shared" si="3"/>
-        <v>d 16</v>
+        <v>d 4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add rank changes field for 1Q 2020
</commit_message>
<xml_diff>
--- a/results/rank-changes.xlsx
+++ b/results/rank-changes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645"/>
   </bookViews>
   <sheets>
     <sheet name="20201Q" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="939" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="137">
   <si>
     <t>Tag</t>
   </si>
@@ -762,823 +762,2034 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B101"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:5">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" t="s">
+        <v>136</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2">
+        <f>VLOOKUP(A2, '2019'!A:B, 2, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(ISNA(D2), "new", IF(D2 = 0, "-", IF(D2 &gt; 0, CONCATENATE("u ", D2),   IF(D2 &lt; 0, CONCATENATE("d ", ABS(D2))))))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
-    </row>
-    <row r="4" spans="1:2">
+      <c r="C3">
+        <f>VLOOKUP(A3, '2019'!A:B, 2, FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E66" si="1">IF(ISNA(D3), "new", IF(D3 = 0, "-", IF(D3 &gt; 0, CONCATENATE("u ", D3),   IF(D3 &lt; 0, CONCATENATE("d ", ABS(D3))))))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:2">
+      <c r="C4">
+        <f>VLOOKUP(A4, '2019'!A:B, 2, FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5">
+        <f>VLOOKUP(A5, '2019'!A:B, 2, FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:2">
+      <c r="C6">
+        <f>VLOOKUP(A6, '2019'!A:B, 2, FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:2">
+      <c r="C7">
+        <f>VLOOKUP(A7, '2019'!A:B, 2, FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
-    </row>
-    <row r="9" spans="1:2">
+      <c r="C8">
+        <f>VLOOKUP(A8, '2019'!A:B, 2, FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
-    </row>
-    <row r="10" spans="1:2">
+      <c r="C9">
+        <f>VLOOKUP(A9, '2019'!A:B, 2, FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
-    </row>
-    <row r="11" spans="1:2">
+      <c r="C10">
+        <f>VLOOKUP(A10, '2019'!A:B, 2, FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
-    </row>
-    <row r="12" spans="1:2">
+      <c r="C11">
+        <f>VLOOKUP(A11, '2019'!A:B, 2, FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" spans="1:2">
+      <c r="C12">
+        <f>VLOOKUP(A12, '2019'!A:B, 2, FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
-    </row>
-    <row r="14" spans="1:2">
+      <c r="C13">
+        <f>VLOOKUP(A13, '2019'!A:B, 2, FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
-    </row>
-    <row r="15" spans="1:2">
+      <c r="C14">
+        <f>VLOOKUP(A14, '2019'!A:B, 2, FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>15</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
+      <c r="C15">
+        <f>VLOOKUP(A15, '2019'!A:B, 2, FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>16</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
-    </row>
-    <row r="17" spans="1:2">
+      <c r="C16">
+        <f>VLOOKUP(A16, '2019'!A:B, 2, FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
-    </row>
-    <row r="18" spans="1:2">
+      <c r="C17">
+        <f>VLOOKUP(A17, '2019'!A:B, 2, FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>18</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
-    </row>
-    <row r="19" spans="1:2">
+      <c r="C18">
+        <f>VLOOKUP(A18, '2019'!A:B, 2, FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>19</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="1:2">
+      <c r="C19">
+        <f>VLOOKUP(A19, '2019'!A:B, 2, FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>20</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
-    </row>
-    <row r="21" spans="1:2">
+      <c r="C20">
+        <f>VLOOKUP(A20, '2019'!A:B, 2, FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>21</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
-    </row>
-    <row r="22" spans="1:2">
+      <c r="C21">
+        <f>VLOOKUP(A21, '2019'!A:B, 2, FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>22</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
-    </row>
-    <row r="23" spans="1:2">
+      <c r="C22">
+        <f>VLOOKUP(A22, '2019'!A:B, 2, FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>23</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
-    </row>
-    <row r="24" spans="1:2">
+      <c r="C23">
+        <f>VLOOKUP(A23, '2019'!A:B, 2, FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>24</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
-    </row>
-    <row r="25" spans="1:2">
+      <c r="C24">
+        <f>VLOOKUP(A24, '2019'!A:B, 2, FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" t="s">
         <v>25</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
-    </row>
-    <row r="26" spans="1:2">
+      <c r="C25">
+        <f>VLOOKUP(A25, '2019'!A:B, 2, FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
       <c r="A26" t="s">
         <v>26</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:2">
+      <c r="C26">
+        <f>VLOOKUP(A26, '2019'!A:B, 2, FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" t="s">
         <v>27</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:2">
+      <c r="C27">
+        <f>VLOOKUP(A27, '2019'!A:B, 2, FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
       <c r="A28" t="s">
         <v>28</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
-    </row>
-    <row r="29" spans="1:2">
+      <c r="C28">
+        <f>VLOOKUP(A28, '2019'!A:B, 2, FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
       <c r="A29" t="s">
         <v>29</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
-    </row>
-    <row r="30" spans="1:2">
+      <c r="C29">
+        <f>VLOOKUP(A29, '2019'!A:B, 2, FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
       <c r="A30" t="s">
         <v>30</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
-    </row>
-    <row r="31" spans="1:2">
+      <c r="C30">
+        <f>VLOOKUP(A30, '2019'!A:B, 2, FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
       <c r="A31" t="s">
         <v>31</v>
       </c>
       <c r="B31">
         <v>30</v>
       </c>
-    </row>
-    <row r="32" spans="1:2">
+      <c r="C31">
+        <f>VLOOKUP(A31, '2019'!A:B, 2, FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
       <c r="A32" t="s">
         <v>32</v>
       </c>
       <c r="B32">
         <v>31</v>
       </c>
-    </row>
-    <row r="33" spans="1:2">
+      <c r="C32">
+        <f>VLOOKUP(A32, '2019'!A:B, 2, FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
       <c r="A33" t="s">
         <v>33</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
-    </row>
-    <row r="34" spans="1:2">
+      <c r="C33">
+        <f>VLOOKUP(A33, '2019'!A:B, 2, FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
       <c r="A34" t="s">
         <v>34</v>
       </c>
       <c r="B34">
         <v>33</v>
       </c>
-    </row>
-    <row r="35" spans="1:2">
+      <c r="C34">
+        <f>VLOOKUP(A34, '2019'!A:B, 2, FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="1"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
       <c r="A35" t="s">
         <v>35</v>
       </c>
       <c r="B35">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
+      <c r="C35">
+        <f>VLOOKUP(A35, '2019'!A:B, 2, FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
       <c r="A36" t="s">
         <v>36</v>
       </c>
       <c r="B36">
         <v>35</v>
       </c>
-    </row>
-    <row r="37" spans="1:2">
+      <c r="C36">
+        <f>VLOOKUP(A36, '2019'!A:B, 2, FALSE)</f>
+        <v>36</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
       <c r="A37" t="s">
         <v>37</v>
       </c>
       <c r="B37">
         <v>36</v>
       </c>
-    </row>
-    <row r="38" spans="1:2">
+      <c r="C37">
+        <f>VLOOKUP(A37, '2019'!A:B, 2, FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
       <c r="A38" t="s">
         <v>38</v>
       </c>
       <c r="B38">
         <v>37</v>
       </c>
-    </row>
-    <row r="39" spans="1:2">
+      <c r="C38">
+        <f>VLOOKUP(A38, '2019'!A:B, 2, FALSE)</f>
+        <v>38</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
       <c r="A39" t="s">
         <v>39</v>
       </c>
       <c r="B39">
         <v>38</v>
       </c>
-    </row>
-    <row r="40" spans="1:2">
+      <c r="C39">
+        <f>VLOOKUP(A39, '2019'!A:B, 2, FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
       <c r="A40" t="s">
         <v>40</v>
       </c>
       <c r="B40">
         <v>39</v>
       </c>
-    </row>
-    <row r="41" spans="1:2">
+      <c r="C40">
+        <f>VLOOKUP(A40, '2019'!A:B, 2, FALSE)</f>
+        <v>37</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
       <c r="A41" t="s">
         <v>41</v>
       </c>
       <c r="B41">
         <v>40</v>
       </c>
-    </row>
-    <row r="42" spans="1:2">
+      <c r="C41">
+        <f>VLOOKUP(A41, '2019'!A:B, 2, FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="1"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
       <c r="A42" t="s">
         <v>42</v>
       </c>
       <c r="B42">
         <v>41</v>
       </c>
-    </row>
-    <row r="43" spans="1:2">
+      <c r="C42">
+        <f>VLOOKUP(A42, '2019'!A:B, 2, FALSE)</f>
+        <v>42</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
       <c r="A43" t="s">
         <v>43</v>
       </c>
       <c r="B43">
         <v>42</v>
       </c>
-    </row>
-    <row r="44" spans="1:2">
+      <c r="C43">
+        <f>VLOOKUP(A43, '2019'!A:B, 2, FALSE)</f>
+        <v>41</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
       <c r="A44" t="s">
         <v>44</v>
       </c>
       <c r="B44">
         <v>43</v>
       </c>
-    </row>
-    <row r="45" spans="1:2">
+      <c r="C44">
+        <f>VLOOKUP(A44, '2019'!A:B, 2, FALSE)</f>
+        <v>44</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" t="s">
         <v>45</v>
       </c>
       <c r="B45">
         <v>44</v>
       </c>
-    </row>
-    <row r="46" spans="1:2">
+      <c r="C45">
+        <f>VLOOKUP(A45, '2019'!A:B, 2, FALSE)</f>
+        <v>47</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" t="s">
         <v>46</v>
       </c>
       <c r="B46">
         <v>45</v>
       </c>
-    </row>
-    <row r="47" spans="1:2">
+      <c r="C46">
+        <f>VLOOKUP(A46, '2019'!A:B, 2, FALSE)</f>
+        <v>52</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="1"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
       <c r="A47" t="s">
         <v>47</v>
       </c>
       <c r="B47">
         <v>46</v>
       </c>
-    </row>
-    <row r="48" spans="1:2">
+      <c r="C47">
+        <f>VLOOKUP(A47, '2019'!A:B, 2, FALSE)</f>
+        <v>56</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="1"/>
+        <v>u 10</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" t="s">
         <v>48</v>
       </c>
       <c r="B48">
         <v>47</v>
       </c>
-    </row>
-    <row r="49" spans="1:2">
+      <c r="C48">
+        <f>VLOOKUP(A48, '2019'!A:B, 2, FALSE)</f>
+        <v>45</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
       <c r="A49" t="s">
         <v>49</v>
       </c>
       <c r="B49">
         <v>48</v>
       </c>
-    </row>
-    <row r="50" spans="1:2">
+      <c r="C49">
+        <f>VLOOKUP(A49, '2019'!A:B, 2, FALSE)</f>
+        <v>43</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
       <c r="A50" t="s">
         <v>50</v>
       </c>
       <c r="B50">
         <v>49</v>
       </c>
-    </row>
-    <row r="51" spans="1:2">
+      <c r="C50">
+        <f>VLOOKUP(A50, '2019'!A:B, 2, FALSE)</f>
+        <v>60</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="1"/>
+        <v>u 11</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
       <c r="A51" t="s">
         <v>51</v>
       </c>
       <c r="B51">
         <v>50</v>
       </c>
-    </row>
-    <row r="52" spans="1:2">
+      <c r="C51">
+        <f>VLOOKUP(A51, '2019'!A:B, 2, FALSE)</f>
+        <v>49</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
       <c r="A52" t="s">
         <v>52</v>
       </c>
       <c r="B52">
         <v>51</v>
       </c>
-    </row>
-    <row r="53" spans="1:2">
+      <c r="C52">
+        <f>VLOOKUP(A52, '2019'!A:B, 2, FALSE)</f>
+        <v>46</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
       <c r="A53" t="s">
         <v>53</v>
       </c>
       <c r="B53">
         <v>52</v>
       </c>
-    </row>
-    <row r="54" spans="1:2">
+      <c r="C53">
+        <f>VLOOKUP(A53, '2019'!A:B, 2, FALSE)</f>
+        <v>55</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
       <c r="A54" t="s">
         <v>54</v>
       </c>
       <c r="B54">
         <v>53</v>
       </c>
-    </row>
-    <row r="55" spans="1:2">
+      <c r="C54">
+        <f>VLOOKUP(A54, '2019'!A:B, 2, FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
       <c r="A55" t="s">
         <v>55</v>
       </c>
       <c r="B55">
         <v>54</v>
       </c>
-    </row>
-    <row r="56" spans="1:2">
+      <c r="C55">
+        <f>VLOOKUP(A55, '2019'!A:B, 2, FALSE)</f>
+        <v>57</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
       <c r="A56" t="s">
         <v>56</v>
       </c>
       <c r="B56">
         <v>55</v>
       </c>
-    </row>
-    <row r="57" spans="1:2">
+      <c r="C56">
+        <f>VLOOKUP(A56, '2019'!A:B, 2, FALSE)</f>
+        <v>51</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>-4</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="1"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
       <c r="A57" t="s">
         <v>57</v>
       </c>
       <c r="B57">
         <v>56</v>
       </c>
-    </row>
-    <row r="58" spans="1:2">
+      <c r="C57">
+        <f>VLOOKUP(A57, '2019'!A:B, 2, FALSE)</f>
+        <v>54</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
       <c r="A58" t="s">
         <v>58</v>
       </c>
       <c r="B58">
         <v>57</v>
       </c>
-    </row>
-    <row r="59" spans="1:2">
+      <c r="C58">
+        <f>VLOOKUP(A58, '2019'!A:B, 2, FALSE)</f>
+        <v>58</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
       <c r="A59" t="s">
         <v>59</v>
       </c>
       <c r="B59">
         <v>58</v>
       </c>
-    </row>
-    <row r="60" spans="1:2">
+      <c r="C59">
+        <f>VLOOKUP(A59, '2019'!A:B, 2, FALSE)</f>
+        <v>48</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>-10</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="1"/>
+        <v>d 10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
       <c r="A60" t="s">
         <v>60</v>
       </c>
       <c r="B60">
         <v>59</v>
       </c>
-    </row>
-    <row r="61" spans="1:2">
+      <c r="C60">
+        <f>VLOOKUP(A60, '2019'!A:B, 2, FALSE)</f>
+        <v>63</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="1"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
       <c r="A61" t="s">
         <v>61</v>
       </c>
       <c r="B61">
         <v>60</v>
       </c>
-    </row>
-    <row r="62" spans="1:2">
+      <c r="C61">
+        <f>VLOOKUP(A61, '2019'!A:B, 2, FALSE)</f>
+        <v>61</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
       <c r="A62" t="s">
         <v>62</v>
       </c>
       <c r="B62">
         <v>61</v>
       </c>
-    </row>
-    <row r="63" spans="1:2">
+      <c r="C62">
+        <f>VLOOKUP(A62, '2019'!A:B, 2, FALSE)</f>
+        <v>53</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
       <c r="A63" t="s">
         <v>63</v>
       </c>
       <c r="B63">
         <v>62</v>
       </c>
-    </row>
-    <row r="64" spans="1:2">
+      <c r="C63">
+        <f>VLOOKUP(A63, '2019'!A:B, 2, FALSE)</f>
+        <v>70</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="1"/>
+        <v>u 8</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
       <c r="A64" t="s">
         <v>64</v>
       </c>
       <c r="B64">
         <v>63</v>
       </c>
-    </row>
-    <row r="65" spans="1:2">
+      <c r="C64">
+        <f>VLOOKUP(A64, '2019'!A:B, 2, FALSE)</f>
+        <v>64</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
       <c r="A65" t="s">
         <v>65</v>
       </c>
       <c r="B65">
         <v>64</v>
       </c>
-    </row>
-    <row r="66" spans="1:2">
+      <c r="C65">
+        <f>VLOOKUP(A65, '2019'!A:B, 2, FALSE)</f>
+        <v>66</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
       <c r="A66" t="s">
         <v>66</v>
       </c>
       <c r="B66">
         <v>65</v>
       </c>
-    </row>
-    <row r="67" spans="1:2">
+      <c r="C66">
+        <f>VLOOKUP(A66, '2019'!A:B, 2, FALSE)</f>
+        <v>81</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="1"/>
+        <v>u 16</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
       <c r="A67" t="s">
         <v>67</v>
       </c>
       <c r="B67">
         <v>66</v>
       </c>
-    </row>
-    <row r="68" spans="1:2">
+      <c r="C67">
+        <f>VLOOKUP(A67, '2019'!A:B, 2, FALSE)</f>
+        <v>62</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D101" si="2">C67-B67</f>
+        <v>-4</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" ref="E67:E101" si="3">IF(ISNA(D67), "new", IF(D67 = 0, "-", IF(D67 &gt; 0, CONCATENATE("u ", D67),   IF(D67 &lt; 0, CONCATENATE("d ", ABS(D67))))))</f>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
       <c r="A68" t="s">
         <v>68</v>
       </c>
       <c r="B68">
         <v>67</v>
       </c>
-    </row>
-    <row r="69" spans="1:2">
+      <c r="C68">
+        <f>VLOOKUP(A68, '2019'!A:B, 2, FALSE)</f>
+        <v>75</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="3"/>
+        <v>u 8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
       <c r="A69" t="s">
         <v>69</v>
       </c>
       <c r="B69">
         <v>68</v>
       </c>
-    </row>
-    <row r="70" spans="1:2">
+      <c r="C69">
+        <f>VLOOKUP(A69, '2019'!A:B, 2, FALSE)</f>
+        <v>74</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="3"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
       <c r="A70" t="s">
         <v>70</v>
       </c>
       <c r="B70">
         <v>69</v>
       </c>
-    </row>
-    <row r="71" spans="1:2">
+      <c r="C70">
+        <f>VLOOKUP(A70, '2019'!A:B, 2, FALSE)</f>
+        <v>59</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="3"/>
+        <v>d 10</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
       <c r="A71" t="s">
         <v>71</v>
       </c>
       <c r="B71">
         <v>70</v>
       </c>
-    </row>
-    <row r="72" spans="1:2">
+      <c r="C71">
+        <f>VLOOKUP(A71, '2019'!A:B, 2, FALSE)</f>
+        <v>73</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="3"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
       <c r="A72" t="s">
         <v>72</v>
       </c>
       <c r="B72">
         <v>72</v>
       </c>
-    </row>
-    <row r="73" spans="1:2">
+      <c r="C72">
+        <f>VLOOKUP(A72, '2019'!A:B, 2, FALSE)</f>
+        <v>78</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="3"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
       <c r="A73" t="s">
         <v>73</v>
       </c>
       <c r="B73">
         <v>71</v>
       </c>
-    </row>
-    <row r="74" spans="1:2">
+      <c r="C73">
+        <f>VLOOKUP(A73, '2019'!A:B, 2, FALSE)</f>
+        <v>76</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
       <c r="A74" t="s">
         <v>74</v>
       </c>
       <c r="B74">
         <v>73</v>
       </c>
-    </row>
-    <row r="75" spans="1:2">
+      <c r="C74">
+        <f>VLOOKUP(A74, '2019'!A:B, 2, FALSE)</f>
+        <v>72</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="3"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
       <c r="A75" t="s">
         <v>75</v>
       </c>
       <c r="B75">
         <v>74</v>
       </c>
-    </row>
-    <row r="76" spans="1:2">
+      <c r="C75">
+        <f>VLOOKUP(A75, '2019'!A:B, 2, FALSE)</f>
+        <v>84</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="3"/>
+        <v>u 10</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
       <c r="A76" t="s">
         <v>76</v>
       </c>
       <c r="B76">
         <v>75</v>
       </c>
-    </row>
-    <row r="77" spans="1:2">
+      <c r="C76">
+        <f>VLOOKUP(A76, '2019'!A:B, 2, FALSE)</f>
+        <v>67</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="3"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
       <c r="A77" t="s">
         <v>77</v>
       </c>
       <c r="B77">
         <v>76</v>
       </c>
-    </row>
-    <row r="78" spans="1:2">
+      <c r="C77">
+        <f>VLOOKUP(A77, '2019'!A:B, 2, FALSE)</f>
+        <v>65</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="2"/>
+        <v>-11</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="3"/>
+        <v>d 11</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
       <c r="A78" t="s">
         <v>78</v>
       </c>
       <c r="B78">
         <v>77</v>
       </c>
-    </row>
-    <row r="79" spans="1:2">
+      <c r="C78">
+        <f>VLOOKUP(A78, '2019'!A:B, 2, FALSE)</f>
+        <v>68</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="3"/>
+        <v>d 9</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
       <c r="A79" t="s">
         <v>79</v>
       </c>
       <c r="B79">
         <v>78</v>
       </c>
-    </row>
-    <row r="80" spans="1:2">
+      <c r="C79">
+        <f>VLOOKUP(A79, '2019'!A:B, 2, FALSE)</f>
+        <v>77</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="3"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
       <c r="A80" t="s">
         <v>80</v>
       </c>
       <c r="B80">
         <v>79</v>
       </c>
-    </row>
-    <row r="81" spans="1:2">
+      <c r="C80">
+        <f>VLOOKUP(A80, '2019'!A:B, 2, FALSE)</f>
+        <v>91</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="2"/>
+        <v>12</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="3"/>
+        <v>u 12</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
       <c r="A81" t="s">
         <v>81</v>
       </c>
       <c r="B81">
         <v>80</v>
       </c>
-    </row>
-    <row r="82" spans="1:2">
+      <c r="C81">
+        <f>VLOOKUP(A81, '2019'!A:B, 2, FALSE)</f>
+        <v>71</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="3"/>
+        <v>d 9</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
       <c r="A82" t="s">
         <v>82</v>
       </c>
       <c r="B82">
         <v>81</v>
       </c>
-    </row>
-    <row r="83" spans="1:2">
+      <c r="C82">
+        <f>VLOOKUP(A82, '2019'!A:B, 2, FALSE)</f>
+        <v>82</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="3"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
       <c r="A83" t="s">
         <v>83</v>
       </c>
       <c r="B83">
         <v>82</v>
       </c>
-    </row>
-    <row r="84" spans="1:2">
+      <c r="C83">
+        <f>VLOOKUP(A83, '2019'!A:B, 2, FALSE)</f>
+        <v>89</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="2"/>
+        <v>7</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="3"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
       <c r="A84" t="s">
         <v>84</v>
       </c>
       <c r="B84">
         <v>83</v>
       </c>
-    </row>
-    <row r="85" spans="1:2">
+      <c r="C84">
+        <f>VLOOKUP(A84, '2019'!A:B, 2, FALSE)</f>
+        <v>83</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
       <c r="A85" t="s">
         <v>85</v>
       </c>
       <c r="B85">
         <v>84</v>
       </c>
-    </row>
-    <row r="86" spans="1:2">
+      <c r="C85">
+        <f>VLOOKUP(A85, '2019'!A:B, 2, FALSE)</f>
+        <v>88</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="3"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
       <c r="A86" t="s">
         <v>86</v>
       </c>
       <c r="B86">
         <v>85</v>
       </c>
-    </row>
-    <row r="87" spans="1:2">
+      <c r="C86">
+        <f>VLOOKUP(A86, '2019'!A:B, 2, FALSE)</f>
+        <v>90</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
       <c r="A87" t="s">
         <v>87</v>
       </c>
       <c r="B87">
         <v>86</v>
       </c>
-    </row>
-    <row r="88" spans="1:2">
+      <c r="C87">
+        <f>VLOOKUP(A87, '2019'!A:B, 2, FALSE)</f>
+        <v>80</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="2"/>
+        <v>-6</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="3"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
       <c r="A88" t="s">
         <v>88</v>
       </c>
       <c r="B88">
         <v>87</v>
       </c>
-    </row>
-    <row r="89" spans="1:2">
+      <c r="C88">
+        <f>VLOOKUP(A88, '2019'!A:B, 2, FALSE)</f>
+        <v>92</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
       <c r="A89" t="s">
         <v>89</v>
       </c>
       <c r="B89">
         <v>88</v>
       </c>
-    </row>
-    <row r="90" spans="1:2">
+      <c r="C89" t="e">
+        <f>VLOOKUP(A89, '2019'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D89" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
       <c r="A90" t="s">
         <v>90</v>
       </c>
       <c r="B90">
         <v>89</v>
       </c>
-    </row>
-    <row r="91" spans="1:2">
+      <c r="C90">
+        <f>VLOOKUP(A90, '2019'!A:B, 2, FALSE)</f>
+        <v>94</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
       <c r="A91" t="s">
         <v>91</v>
       </c>
       <c r="B91">
         <v>90</v>
       </c>
-    </row>
-    <row r="92" spans="1:2">
+      <c r="C91">
+        <f>VLOOKUP(A91, '2019'!A:B, 2, FALSE)</f>
+        <v>95</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
       <c r="A92" t="s">
         <v>92</v>
       </c>
       <c r="B92">
         <v>91</v>
       </c>
-    </row>
-    <row r="93" spans="1:2">
+      <c r="C92">
+        <f>VLOOKUP(A92, '2019'!A:B, 2, FALSE)</f>
+        <v>87</v>
+      </c>
+      <c r="D92">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="3"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
       <c r="A93" t="s">
         <v>93</v>
       </c>
       <c r="B93">
         <v>92</v>
       </c>
-    </row>
-    <row r="94" spans="1:2">
+      <c r="C93" t="e">
+        <f>VLOOKUP(A93, '2019'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D93" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
       <c r="A94" t="s">
         <v>94</v>
       </c>
       <c r="B94">
         <v>93</v>
       </c>
-    </row>
-    <row r="95" spans="1:2">
+      <c r="C94">
+        <f>VLOOKUP(A94, '2019'!A:B, 2, FALSE)</f>
+        <v>86</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="2"/>
+        <v>-7</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="3"/>
+        <v>d 7</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
       <c r="A95" t="s">
         <v>95</v>
       </c>
       <c r="B95">
         <v>94</v>
       </c>
-    </row>
-    <row r="96" spans="1:2">
+      <c r="C95">
+        <f>VLOOKUP(A95, '2019'!A:B, 2, FALSE)</f>
+        <v>69</v>
+      </c>
+      <c r="D95">
+        <f t="shared" si="2"/>
+        <v>-25</v>
+      </c>
+      <c r="E95" t="str">
+        <f t="shared" si="3"/>
+        <v>d 25</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
       <c r="A96" t="s">
         <v>96</v>
       </c>
       <c r="B96">
         <v>95</v>
       </c>
-    </row>
-    <row r="97" spans="1:2">
+      <c r="C96">
+        <f>VLOOKUP(A96, '2019'!A:B, 2, FALSE)</f>
+        <v>85</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="3"/>
+        <v>d 10</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
       <c r="A97" t="s">
         <v>97</v>
       </c>
       <c r="B97">
         <v>96</v>
       </c>
-    </row>
-    <row r="98" spans="1:2">
+      <c r="C97">
+        <f>VLOOKUP(A97, '2019'!A:B, 2, FALSE)</f>
+        <v>97</v>
+      </c>
+      <c r="D97">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="3"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
       <c r="A98" t="s">
         <v>98</v>
       </c>
       <c r="B98">
         <v>97</v>
       </c>
-    </row>
-    <row r="99" spans="1:2">
+      <c r="C98">
+        <f>VLOOKUP(A98, '2019'!A:B, 2, FALSE)</f>
+        <v>79</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="2"/>
+        <v>-18</v>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="3"/>
+        <v>d 18</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
       <c r="A99" t="s">
         <v>99</v>
       </c>
       <c r="B99">
         <v>98</v>
       </c>
-    </row>
-    <row r="100" spans="1:2">
+      <c r="C99">
+        <f>VLOOKUP(A99, '2019'!A:B, 2, FALSE)</f>
+        <v>96</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="3"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
       <c r="A100" t="s">
         <v>100</v>
       </c>
       <c r="B100">
         <v>99</v>
       </c>
-    </row>
-    <row r="101" spans="1:2">
+      <c r="C100" t="e">
+        <f>VLOOKUP(A100, '2019'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D100" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
       <c r="A101" t="s">
         <v>101</v>
       </c>
       <c r="B101">
         <v>100</v>
+      </c>
+      <c r="C101" t="e">
+        <f>VLOOKUP(A101, '2019'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D101" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
       </c>
     </row>
   </sheetData>
@@ -14652,8 +15863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Add Most popular StackOverflow tags in 2021
</commit_message>
<xml_diff>
--- a/results/rank-changes.xlsx
+++ b/results/rank-changes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="9645" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="20201Q" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="942" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="138">
   <si>
     <t>Tag</t>
   </si>
@@ -445,6 +445,9 @@
   <si>
     <t>Rank 2019</t>
   </si>
+  <si>
+    <t>Rank 2020</t>
+  </si>
 </sst>
 </file>
 
@@ -764,7 +767,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -2799,12 +2802,2037 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E101"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" t="s">
+        <v>108</v>
+      </c>
+      <c r="E1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <f>VLOOKUP(A2, '2020'!A:B, 2, FALSE)</f>
+        <v>1</v>
+      </c>
+      <c r="D2">
+        <f>C2-B2</f>
+        <v>0</v>
+      </c>
+      <c r="E2" t="str">
+        <f>IF(ISNA(D2), "new", IF(D2 = 0, "-", IF(D2 &gt; 0, CONCATENATE("u ", D2),   IF(D2 &lt; 0, CONCATENATE("d ", ABS(D2))))))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <f>VLOOKUP(A3, '2020'!A:B, 2, FALSE)</f>
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D66" si="0">C3-B3</f>
+        <v>0</v>
+      </c>
+      <c r="E3" t="str">
+        <f t="shared" ref="E3:E66" si="1">IF(ISNA(D3), "new", IF(D3 = 0, "-", IF(D3 &gt; 0, CONCATENATE("u ", D3),   IF(D3 &lt; 0, CONCATENATE("d ", ABS(D3))))))</f>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <f>VLOOKUP(A4, '2020'!A:B, 2, FALSE)</f>
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E4" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5">
+        <f>VLOOKUP(A5, '2020'!A:B, 2, FALSE)</f>
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E5" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <f>VLOOKUP(A6, '2020'!A:B, 2, FALSE)</f>
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E6" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7">
+        <f>VLOOKUP(A7, '2020'!A:B, 2, FALSE)</f>
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E7" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8">
+        <f>VLOOKUP(A8, '2020'!A:B, 2, FALSE)</f>
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E8" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9">
+        <f>VLOOKUP(A9, '2020'!A:B, 2, FALSE)</f>
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E9" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <f>VLOOKUP(A10, '2020'!A:B, 2, FALSE)</f>
+        <v>8</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E10" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11">
+        <f>VLOOKUP(A11, '2020'!A:B, 2, FALSE)</f>
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E11" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12">
+        <f>VLOOKUP(A12, '2020'!A:B, 2, FALSE)</f>
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E12" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <f>VLOOKUP(A13, '2020'!A:B, 2, FALSE)</f>
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E13" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14">
+        <f>VLOOKUP(A14, '2020'!A:B, 2, FALSE)</f>
+        <v>12</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E14" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <f>VLOOKUP(A15, '2020'!A:B, 2, FALSE)</f>
+        <v>15</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E15" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16">
+        <f>VLOOKUP(A16, '2020'!A:B, 2, FALSE)</f>
+        <v>14</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E16" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17">
+        <f>VLOOKUP(A17, '2020'!A:B, 2, FALSE)</f>
+        <v>17</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E17" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18">
+        <f>VLOOKUP(A18, '2020'!A:B, 2, FALSE)</f>
+        <v>16</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E18" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19">
+        <f>VLOOKUP(A19, '2020'!A:B, 2, FALSE)</f>
+        <v>19</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E19" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <f>VLOOKUP(A20, '2020'!A:B, 2, FALSE)</f>
+        <v>21</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E20" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <f>VLOOKUP(A21, '2020'!A:B, 2, FALSE)</f>
+        <v>18</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E21" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <f>VLOOKUP(A22, '2020'!A:B, 2, FALSE)</f>
+        <v>20</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E22" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>26</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <f>VLOOKUP(A23, '2020'!A:B, 2, FALSE)</f>
+        <v>25</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E23" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <f>VLOOKUP(A24, '2020'!A:B, 2, FALSE)</f>
+        <v>22</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E24" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <f>VLOOKUP(A25, '2020'!A:B, 2, FALSE)</f>
+        <v>26</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E25" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <f>VLOOKUP(A26, '2020'!A:B, 2, FALSE)</f>
+        <v>23</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E26" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <f>VLOOKUP(A27, '2020'!A:B, 2, FALSE)</f>
+        <v>31</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E27" t="str">
+        <f t="shared" si="1"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B28">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <f>VLOOKUP(A28, '2020'!A:B, 2, FALSE)</f>
+        <v>24</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E28" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>32</v>
+      </c>
+      <c r="B29">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <f>VLOOKUP(A29, '2020'!A:B, 2, FALSE)</f>
+        <v>28</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E29" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <f>VLOOKUP(A30, '2020'!A:B, 2, FALSE)</f>
+        <v>27</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E30" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <f>VLOOKUP(A31, '2020'!A:B, 2, FALSE)</f>
+        <v>30</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E31" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32">
+        <v>31</v>
+      </c>
+      <c r="C32">
+        <f>VLOOKUP(A32, '2020'!A:B, 2, FALSE)</f>
+        <v>33</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E32" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5">
+      <c r="A33" t="s">
+        <v>28</v>
+      </c>
+      <c r="B33">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <f>VLOOKUP(A33, '2020'!A:B, 2, FALSE)</f>
+        <v>29</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E33" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5">
+      <c r="A34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B34">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <f>VLOOKUP(A34, '2020'!A:B, 2, FALSE)</f>
+        <v>32</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E34" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <f>VLOOKUP(A35, '2020'!A:B, 2, FALSE)</f>
+        <v>36</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="E35" t="str">
+        <f t="shared" si="1"/>
+        <v>u 2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5">
+      <c r="A36" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <f>VLOOKUP(A36, '2020'!A:B, 2, FALSE)</f>
+        <v>34</v>
+      </c>
+      <c r="D36">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E36" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5">
+      <c r="A37" t="s">
+        <v>50</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37">
+        <f>VLOOKUP(A37, '2020'!A:B, 2, FALSE)</f>
+        <v>41</v>
+      </c>
+      <c r="D37">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="E37" t="str">
+        <f t="shared" si="1"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5">
+      <c r="A38" t="s">
+        <v>39</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38">
+        <f>VLOOKUP(A38, '2020'!A:B, 2, FALSE)</f>
+        <v>37</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E38" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5">
+      <c r="A39" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39">
+        <f>VLOOKUP(A39, '2020'!A:B, 2, FALSE)</f>
+        <v>38</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E39" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5">
+      <c r="A40" t="s">
+        <v>44</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40">
+        <f>VLOOKUP(A40, '2020'!A:B, 2, FALSE)</f>
+        <v>42</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E40" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5">
+      <c r="A41" t="s">
+        <v>30</v>
+      </c>
+      <c r="B41">
+        <v>40</v>
+      </c>
+      <c r="C41">
+        <f>VLOOKUP(A41, '2020'!A:B, 2, FALSE)</f>
+        <v>35</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E41" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42">
+        <v>41</v>
+      </c>
+      <c r="C42">
+        <f>VLOOKUP(A42, '2020'!A:B, 2, FALSE)</f>
+        <v>49</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="E42" t="str">
+        <f t="shared" si="1"/>
+        <v>u 8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43">
+        <v>42</v>
+      </c>
+      <c r="C43">
+        <f>VLOOKUP(A43, '2020'!A:B, 2, FALSE)</f>
+        <v>39</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="0"/>
+        <v>-3</v>
+      </c>
+      <c r="E43" t="str">
+        <f t="shared" si="1"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44">
+        <v>43</v>
+      </c>
+      <c r="C44">
+        <f>VLOOKUP(A44, '2020'!A:B, 2, FALSE)</f>
+        <v>43</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E44" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5">
+      <c r="A45" t="s">
+        <v>46</v>
+      </c>
+      <c r="B45">
+        <v>44</v>
+      </c>
+      <c r="C45">
+        <f>VLOOKUP(A45, '2020'!A:B, 2, FALSE)</f>
+        <v>45</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E45" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" t="s">
+        <v>35</v>
+      </c>
+      <c r="B46">
+        <v>45</v>
+      </c>
+      <c r="C46">
+        <f>VLOOKUP(A46, '2020'!A:B, 2, FALSE)</f>
+        <v>40</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E46" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5">
+      <c r="A47" t="s">
+        <v>63</v>
+      </c>
+      <c r="B47">
+        <v>46</v>
+      </c>
+      <c r="C47">
+        <f>VLOOKUP(A47, '2020'!A:B, 2, FALSE)</f>
+        <v>53</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="E47" t="str">
+        <f t="shared" si="1"/>
+        <v>u 7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48">
+        <v>47</v>
+      </c>
+      <c r="C48">
+        <f>VLOOKUP(A48, '2020'!A:B, 2, FALSE)</f>
+        <v>46</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E48" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49">
+        <v>48</v>
+      </c>
+      <c r="C49">
+        <f>VLOOKUP(A49, '2020'!A:B, 2, FALSE)</f>
+        <v>47</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E49" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50">
+        <v>49</v>
+      </c>
+      <c r="C50">
+        <f>VLOOKUP(A50, '2020'!A:B, 2, FALSE)</f>
+        <v>50</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E50" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5">
+      <c r="A51" t="s">
+        <v>60</v>
+      </c>
+      <c r="B51">
+        <v>50</v>
+      </c>
+      <c r="C51">
+        <f>VLOOKUP(A51, '2020'!A:B, 2, FALSE)</f>
+        <v>54</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E51" t="str">
+        <f t="shared" si="1"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5">
+      <c r="A52" t="s">
+        <v>66</v>
+      </c>
+      <c r="B52">
+        <v>51</v>
+      </c>
+      <c r="C52">
+        <f>VLOOKUP(A52, '2020'!A:B, 2, FALSE)</f>
+        <v>57</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="E52" t="str">
+        <f t="shared" si="1"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5">
+      <c r="A53" t="s">
+        <v>48</v>
+      </c>
+      <c r="B53">
+        <v>52</v>
+      </c>
+      <c r="C53">
+        <f>VLOOKUP(A53, '2020'!A:B, 2, FALSE)</f>
+        <v>52</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E53" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5">
+      <c r="A54" t="s">
+        <v>61</v>
+      </c>
+      <c r="B54">
+        <v>53</v>
+      </c>
+      <c r="C54">
+        <f>VLOOKUP(A54, '2020'!A:B, 2, FALSE)</f>
+        <v>56</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="E54" t="str">
+        <f t="shared" si="1"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" t="s">
+        <v>45</v>
+      </c>
+      <c r="B55">
+        <v>54</v>
+      </c>
+      <c r="C55">
+        <f>VLOOKUP(A55, '2020'!A:B, 2, FALSE)</f>
+        <v>48</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="0"/>
+        <v>-6</v>
+      </c>
+      <c r="E55" t="str">
+        <f t="shared" si="1"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" t="s">
+        <v>90</v>
+      </c>
+      <c r="B56">
+        <v>55</v>
+      </c>
+      <c r="C56">
+        <f>VLOOKUP(A56, '2020'!A:B, 2, FALSE)</f>
+        <v>70</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="E56" t="str">
+        <f t="shared" si="1"/>
+        <v>u 15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" t="s">
+        <v>41</v>
+      </c>
+      <c r="B57">
+        <v>56</v>
+      </c>
+      <c r="C57">
+        <f>VLOOKUP(A57, '2020'!A:B, 2, FALSE)</f>
+        <v>44</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="0"/>
+        <v>-12</v>
+      </c>
+      <c r="E57" t="str">
+        <f t="shared" si="1"/>
+        <v>d 12</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58">
+        <v>57</v>
+      </c>
+      <c r="C58">
+        <f>VLOOKUP(A58, '2020'!A:B, 2, FALSE)</f>
+        <v>55</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="0"/>
+        <v>-2</v>
+      </c>
+      <c r="E58" t="str">
+        <f t="shared" si="1"/>
+        <v>d 2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5">
+      <c r="A59" t="s">
+        <v>57</v>
+      </c>
+      <c r="B59">
+        <v>58</v>
+      </c>
+      <c r="C59">
+        <f>VLOOKUP(A59, '2020'!A:B, 2, FALSE)</f>
+        <v>59</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="E59" t="str">
+        <f t="shared" si="1"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5">
+      <c r="A60" t="s">
+        <v>53</v>
+      </c>
+      <c r="B60">
+        <v>59</v>
+      </c>
+      <c r="C60">
+        <f>VLOOKUP(A60, '2020'!A:B, 2, FALSE)</f>
+        <v>51</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="0"/>
+        <v>-8</v>
+      </c>
+      <c r="E60" t="str">
+        <f t="shared" si="1"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5">
+      <c r="A61" t="s">
+        <v>64</v>
+      </c>
+      <c r="B61">
+        <v>60</v>
+      </c>
+      <c r="C61">
+        <f>VLOOKUP(A61, '2020'!A:B, 2, FALSE)</f>
+        <v>64</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="E61" t="str">
+        <f t="shared" si="1"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5">
+      <c r="A62" t="s">
+        <v>58</v>
+      </c>
+      <c r="B62">
+        <v>61</v>
+      </c>
+      <c r="C62">
+        <f>VLOOKUP(A62, '2020'!A:B, 2, FALSE)</f>
+        <v>61</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E62" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5">
+      <c r="A63" t="s">
+        <v>65</v>
+      </c>
+      <c r="B63">
+        <v>62</v>
+      </c>
+      <c r="C63">
+        <f>VLOOKUP(A63, '2020'!A:B, 2, FALSE)</f>
+        <v>62</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="E63" t="str">
+        <f t="shared" si="1"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5">
+      <c r="A64" t="s">
+        <v>56</v>
+      </c>
+      <c r="B64">
+        <v>63</v>
+      </c>
+      <c r="C64">
+        <f>VLOOKUP(A64, '2020'!A:B, 2, FALSE)</f>
+        <v>58</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E64" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5">
+      <c r="A65" t="s">
+        <v>71</v>
+      </c>
+      <c r="B65">
+        <v>64</v>
+      </c>
+      <c r="C65">
+        <f>VLOOKUP(A65, '2020'!A:B, 2, FALSE)</f>
+        <v>63</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
+      <c r="E65" t="str">
+        <f t="shared" si="1"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5">
+      <c r="A66" t="s">
+        <v>54</v>
+      </c>
+      <c r="B66">
+        <v>65</v>
+      </c>
+      <c r="C66">
+        <f>VLOOKUP(A66, '2020'!A:B, 2, FALSE)</f>
+        <v>60</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="0"/>
+        <v>-5</v>
+      </c>
+      <c r="E66" t="str">
+        <f t="shared" si="1"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5">
+      <c r="A67" t="s">
+        <v>72</v>
+      </c>
+      <c r="B67">
+        <v>66</v>
+      </c>
+      <c r="C67">
+        <f>VLOOKUP(A67, '2020'!A:B, 2, FALSE)</f>
+        <v>65</v>
+      </c>
+      <c r="D67">
+        <f t="shared" ref="D67:D101" si="2">C67-B67</f>
+        <v>-1</v>
+      </c>
+      <c r="E67" t="str">
+        <f t="shared" ref="E67:E101" si="3">IF(ISNA(D67), "new", IF(D67 = 0, "-", IF(D67 &gt; 0, CONCATENATE("u ", D67),   IF(D67 &lt; 0, CONCATENATE("d ", ABS(D67))))))</f>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5">
+      <c r="A68" t="s">
+        <v>89</v>
+      </c>
+      <c r="B68">
+        <v>67</v>
+      </c>
+      <c r="C68">
+        <f>VLOOKUP(A68, '2020'!A:B, 2, FALSE)</f>
+        <v>75</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E68" t="str">
+        <f t="shared" si="3"/>
+        <v>u 8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="A69" t="s">
+        <v>86</v>
+      </c>
+      <c r="B69">
+        <v>68</v>
+      </c>
+      <c r="C69">
+        <f>VLOOKUP(A69, '2020'!A:B, 2, FALSE)</f>
+        <v>72</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E69" t="str">
+        <f t="shared" si="3"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5">
+      <c r="A70" t="s">
+        <v>67</v>
+      </c>
+      <c r="B70">
+        <v>69</v>
+      </c>
+      <c r="C70">
+        <f>VLOOKUP(A70, '2020'!A:B, 2, FALSE)</f>
+        <v>68</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E70" t="str">
+        <f t="shared" si="3"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5">
+      <c r="A71" t="s">
+        <v>62</v>
+      </c>
+      <c r="B71">
+        <v>70</v>
+      </c>
+      <c r="C71">
+        <f>VLOOKUP(A71, '2020'!A:B, 2, FALSE)</f>
+        <v>67</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="E71" t="str">
+        <f t="shared" si="3"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5">
+      <c r="A72" t="s">
+        <v>59</v>
+      </c>
+      <c r="B72">
+        <v>71</v>
+      </c>
+      <c r="C72">
+        <f>VLOOKUP(A72, '2020'!A:B, 2, FALSE)</f>
+        <v>66</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="2"/>
+        <v>-5</v>
+      </c>
+      <c r="E72" t="str">
+        <f t="shared" si="3"/>
+        <v>d 5</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5">
+      <c r="A73" t="s">
+        <v>91</v>
+      </c>
+      <c r="B73">
+        <v>72</v>
+      </c>
+      <c r="C73">
+        <f>VLOOKUP(A73, '2020'!A:B, 2, FALSE)</f>
+        <v>77</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E73" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5">
+      <c r="A74" t="s">
+        <v>80</v>
+      </c>
+      <c r="B74">
+        <v>73</v>
+      </c>
+      <c r="C74">
+        <f>VLOOKUP(A74, '2020'!A:B, 2, FALSE)</f>
+        <v>88</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
+      <c r="E74" t="str">
+        <f t="shared" si="3"/>
+        <v>u 15</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5">
+      <c r="A75" t="s">
+        <v>73</v>
+      </c>
+      <c r="B75">
+        <v>74</v>
+      </c>
+      <c r="C75">
+        <f>VLOOKUP(A75, '2020'!A:B, 2, FALSE)</f>
+        <v>71</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="2"/>
+        <v>-3</v>
+      </c>
+      <c r="E75" t="str">
+        <f t="shared" si="3"/>
+        <v>d 3</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5">
+      <c r="A76" t="s">
+        <v>77</v>
+      </c>
+      <c r="B76">
+        <v>75</v>
+      </c>
+      <c r="C76">
+        <f>VLOOKUP(A76, '2020'!A:B, 2, FALSE)</f>
+        <v>76</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E76" t="str">
+        <f t="shared" si="3"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5">
+      <c r="A77" t="s">
+        <v>92</v>
+      </c>
+      <c r="B77">
+        <v>76</v>
+      </c>
+      <c r="C77">
+        <f>VLOOKUP(A77, '2020'!A:B, 2, FALSE)</f>
+        <v>84</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="2"/>
+        <v>8</v>
+      </c>
+      <c r="E77" t="str">
+        <f t="shared" si="3"/>
+        <v>u 8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5">
+      <c r="A78" t="s">
+        <v>79</v>
+      </c>
+      <c r="B78">
+        <v>77</v>
+      </c>
+      <c r="C78">
+        <f>VLOOKUP(A78, '2020'!A:B, 2, FALSE)</f>
+        <v>81</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="E78" t="str">
+        <f t="shared" si="3"/>
+        <v>u 4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5">
+      <c r="A79" t="s">
+        <v>74</v>
+      </c>
+      <c r="B79">
+        <v>78</v>
+      </c>
+      <c r="C79">
+        <f>VLOOKUP(A79, '2020'!A:B, 2, FALSE)</f>
+        <v>74</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="2"/>
+        <v>-4</v>
+      </c>
+      <c r="E79" t="str">
+        <f t="shared" si="3"/>
+        <v>d 4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5">
+      <c r="A80" t="s">
+        <v>83</v>
+      </c>
+      <c r="B80">
+        <v>79</v>
+      </c>
+      <c r="C80">
+        <f>VLOOKUP(A80, '2020'!A:B, 2, FALSE)</f>
+        <v>80</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E80" t="str">
+        <f t="shared" si="3"/>
+        <v>u 1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5">
+      <c r="A81" t="s">
+        <v>85</v>
+      </c>
+      <c r="B81">
+        <v>80</v>
+      </c>
+      <c r="C81">
+        <f>VLOOKUP(A81, '2020'!A:B, 2, FALSE)</f>
+        <v>83</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="E81" t="str">
+        <f t="shared" si="3"/>
+        <v>u 3</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5">
+      <c r="A82" t="s">
+        <v>69</v>
+      </c>
+      <c r="B82">
+        <v>81</v>
+      </c>
+      <c r="C82">
+        <f>VLOOKUP(A82, '2020'!A:B, 2, FALSE)</f>
+        <v>69</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="2"/>
+        <v>-12</v>
+      </c>
+      <c r="E82" t="str">
+        <f t="shared" si="3"/>
+        <v>d 12</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5">
+      <c r="A83" t="s">
+        <v>104</v>
+      </c>
+      <c r="B83">
+        <v>82</v>
+      </c>
+      <c r="C83" t="e">
+        <f>VLOOKUP(A83, '2020'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D83" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E83" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5">
+      <c r="A84" t="s">
+        <v>103</v>
+      </c>
+      <c r="B84">
+        <v>83</v>
+      </c>
+      <c r="C84">
+        <f>VLOOKUP(A84, '2020'!A:B, 2, FALSE)</f>
+        <v>93</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+      <c r="E84" t="str">
+        <f t="shared" si="3"/>
+        <v>u 10</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5">
+      <c r="A85" t="s">
+        <v>87</v>
+      </c>
+      <c r="B85">
+        <v>84</v>
+      </c>
+      <c r="C85">
+        <f>VLOOKUP(A85, '2020'!A:B, 2, FALSE)</f>
+        <v>90</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="2"/>
+        <v>6</v>
+      </c>
+      <c r="E85" t="str">
+        <f t="shared" si="3"/>
+        <v>u 6</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5">
+      <c r="A86" t="s">
+        <v>122</v>
+      </c>
+      <c r="B86">
+        <v>85</v>
+      </c>
+      <c r="C86" t="e">
+        <f>VLOOKUP(A86, '2020'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D86" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E86" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5">
+      <c r="A87" t="s">
+        <v>70</v>
+      </c>
+      <c r="B87">
+        <v>86</v>
+      </c>
+      <c r="C87">
+        <f>VLOOKUP(A87, '2020'!A:B, 2, FALSE)</f>
+        <v>78</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="2"/>
+        <v>-8</v>
+      </c>
+      <c r="E87" t="str">
+        <f t="shared" si="3"/>
+        <v>d 8</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5">
+      <c r="A88" t="s">
+        <v>68</v>
+      </c>
+      <c r="B88">
+        <v>87</v>
+      </c>
+      <c r="C88">
+        <f>VLOOKUP(A88, '2020'!A:B, 2, FALSE)</f>
+        <v>73</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="2"/>
+        <v>-14</v>
+      </c>
+      <c r="E88" t="str">
+        <f t="shared" si="3"/>
+        <v>d 14</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5">
+      <c r="A89" t="s">
+        <v>82</v>
+      </c>
+      <c r="B89">
+        <v>88</v>
+      </c>
+      <c r="C89">
+        <f>VLOOKUP(A89, '2020'!A:B, 2, FALSE)</f>
+        <v>82</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="2"/>
+        <v>-6</v>
+      </c>
+      <c r="E89" t="str">
+        <f t="shared" si="3"/>
+        <v>d 6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5">
+      <c r="A90" t="s">
+        <v>88</v>
+      </c>
+      <c r="B90">
+        <v>90</v>
+      </c>
+      <c r="C90">
+        <f>VLOOKUP(A90, '2020'!A:B, 2, FALSE)</f>
+        <v>95</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="E90" t="str">
+        <f t="shared" si="3"/>
+        <v>u 5</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5">
+      <c r="A91" t="s">
+        <v>100</v>
+      </c>
+      <c r="B91">
+        <v>89</v>
+      </c>
+      <c r="C91">
+        <f>VLOOKUP(A91, '2020'!A:B, 2, FALSE)</f>
+        <v>89</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E91" t="str">
+        <f t="shared" si="3"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5">
+      <c r="A92" t="s">
+        <v>118</v>
+      </c>
+      <c r="B92">
+        <v>91</v>
+      </c>
+      <c r="C92" t="e">
+        <f>VLOOKUP(A92, '2020'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D92" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E92" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5">
+      <c r="A93" t="s">
+        <v>95</v>
+      </c>
+      <c r="B93">
+        <v>92</v>
+      </c>
+      <c r="C93">
+        <f>VLOOKUP(A93, '2020'!A:B, 2, FALSE)</f>
+        <v>85</v>
+      </c>
+      <c r="D93">
+        <f t="shared" si="2"/>
+        <v>-7</v>
+      </c>
+      <c r="E93" t="str">
+        <f t="shared" si="3"/>
+        <v>d 7</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5">
+      <c r="A94" t="s">
+        <v>84</v>
+      </c>
+      <c r="B94">
+        <v>93</v>
+      </c>
+      <c r="C94">
+        <f>VLOOKUP(A94, '2020'!A:B, 2, FALSE)</f>
+        <v>79</v>
+      </c>
+      <c r="D94">
+        <f t="shared" si="2"/>
+        <v>-14</v>
+      </c>
+      <c r="E94" t="str">
+        <f t="shared" si="3"/>
+        <v>d 14</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5">
+      <c r="A95" t="s">
+        <v>112</v>
+      </c>
+      <c r="B95">
+        <v>94</v>
+      </c>
+      <c r="C95" t="e">
+        <f>VLOOKUP(A95, '2020'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D95" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E95" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5">
+      <c r="A96" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96">
+        <v>95</v>
+      </c>
+      <c r="C96">
+        <f>VLOOKUP(A96, '2020'!A:B, 2, FALSE)</f>
+        <v>86</v>
+      </c>
+      <c r="D96">
+        <f t="shared" si="2"/>
+        <v>-9</v>
+      </c>
+      <c r="E96" t="str">
+        <f t="shared" si="3"/>
+        <v>d 9</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5">
+      <c r="A97" t="s">
+        <v>110</v>
+      </c>
+      <c r="B97">
+        <v>96</v>
+      </c>
+      <c r="C97" t="e">
+        <f>VLOOKUP(A97, '2020'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D97" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E97" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5">
+      <c r="A98" t="s">
+        <v>75</v>
+      </c>
+      <c r="B98">
+        <v>97</v>
+      </c>
+      <c r="C98">
+        <f>VLOOKUP(A98, '2020'!A:B, 2, FALSE)</f>
+        <v>87</v>
+      </c>
+      <c r="D98">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
+      <c r="E98" t="str">
+        <f t="shared" si="3"/>
+        <v>d 10</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5">
+      <c r="A99" t="s">
+        <v>102</v>
+      </c>
+      <c r="B99">
+        <v>98</v>
+      </c>
+      <c r="C99">
+        <f>VLOOKUP(A99, '2020'!A:B, 2, FALSE)</f>
+        <v>97</v>
+      </c>
+      <c r="D99">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="E99" t="str">
+        <f t="shared" si="3"/>
+        <v>d 1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5">
+      <c r="A100" t="s">
+        <v>120</v>
+      </c>
+      <c r="B100">
+        <v>99</v>
+      </c>
+      <c r="C100" t="e">
+        <f>VLOOKUP(A100, '2020'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D100" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E100" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5">
+      <c r="A101" t="s">
+        <v>114</v>
+      </c>
+      <c r="B101">
+        <v>100</v>
+      </c>
+      <c r="C101" t="e">
+        <f>VLOOKUP(A101, '2020'!A:B, 2, FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="D101" t="e">
+        <f t="shared" si="2"/>
+        <v>#N/A</v>
+      </c>
+      <c r="E101" t="str">
+        <f t="shared" si="3"/>
+        <v>new</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>